<commit_message>
Updated new XML samples and mapping
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="660" windowWidth="33760" windowHeight="16060"/>
+    <workbookView xWindow="8520" yWindow="2000" windowWidth="32260" windowHeight="14200"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="310">
   <si>
     <t>Description</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Style</t>
   </si>
   <si>
-    <t>Violation Date</t>
-  </si>
-  <si>
     <t>Municipality</t>
   </si>
   <si>
@@ -144,18 +141,9 @@
     <t>Hazardous Material</t>
   </si>
   <si>
-    <t>Municipal Ordinance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSA </t>
-  </si>
-  <si>
     <t xml:space="preserve">CFR </t>
   </si>
   <si>
-    <t>Violation Code</t>
-  </si>
-  <si>
     <t>POINTS</t>
   </si>
   <si>
@@ -171,12 +159,6 @@
     <t>Date Served</t>
   </si>
   <si>
-    <t>In Hand</t>
-  </si>
-  <si>
-    <t>US Mail</t>
-  </si>
-  <si>
     <t>Officer Name</t>
   </si>
   <si>
@@ -222,9 +204,6 @@
     <t>Vehicle ID</t>
   </si>
   <si>
-    <t>The date the incident occurred</t>
-  </si>
-  <si>
     <t>A landmark or milemarker close to where the incident occurred</t>
   </si>
   <si>
@@ -330,9 +309,6 @@
     <t>Incident number</t>
   </si>
   <si>
-    <t>Incident  Date/Time</t>
-  </si>
-  <si>
     <t>Incident Municipality</t>
   </si>
   <si>
@@ -411,9 +387,6 @@
     <t>Buffalo</t>
   </si>
   <si>
-    <t>5'07"</t>
-  </si>
-  <si>
     <t>BRO</t>
   </si>
   <si>
@@ -447,9 +420,6 @@
     <t>20-124</t>
   </si>
   <si>
-    <t>23V301</t>
-  </si>
-  <si>
     <t>23CFR655</t>
   </si>
   <si>
@@ -501,9 +471,6 @@
     <t>CFR Statute Code</t>
   </si>
   <si>
-    <t>State Statute Code</t>
-  </si>
-  <si>
     <t>Related Criminal Charge Indicator</t>
   </si>
   <si>
@@ -576,9 +543,6 @@
     <t>The 'other' answer provided by the subject</t>
   </si>
   <si>
-    <t>State Statute in violation</t>
-  </si>
-  <si>
     <t>Indicates that there is a related criminal charge</t>
   </si>
   <si>
@@ -588,10 +552,6 @@
     <t>Posteds peed unit of measure</t>
   </si>
   <si>
-    <t>eCitation Element
-(Elements in RED are OJB extensions to the base Incident)</t>
-  </si>
-  <si>
     <t>Vermont eCitation Element</t>
   </si>
   <si>
@@ -616,108 +576,18 @@
     <t>Indicates that thecitation/citation was mailed to the subject.</t>
   </si>
   <si>
-    <t>LICENSE</t>
-  </si>
-  <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ItemModelYearDate</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationJurisdictionFIPS10-4Code</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleMakeCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleColorPrimaryCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleStyleCode</t>
-  </si>
-  <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document[@s:id= /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation/lexslib:SameAsDigestReference/@lexslib:ref]/nc:DocumentIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/j:PersonAugmentation/nc:DriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/j:PersonAugmentation/nc:DriverLicense/j:IdentificationJurisdictionNCICLISCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonSexCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasurePointValue</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:LengthUnitCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasurePointValue</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:WeightUnitCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHairColorCode</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonEyeColorCode</t>
-  </si>
-  <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:EnforcementOfficial/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonFullName</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ActivityInvolvedOrganizationAssociation/nc:OrganizationReference/@s:ref]/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/j:DrivingIncidentRecordedSpeedRate/nc:MeasurePointValue</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/inc-ext:SubjectBloodAlcoholContentNumber</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/j:DrivingIncidentLegalSpeedRate/nc:MeasureUnitText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/j:DrivingIncidentLegalSpeedRate/nc:MeasurePointValue</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/inc-ext:DrivingAccidentIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/inc-ext:DrivingAccidentFatalityIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/inc-ext:SeatBeltViolationIndicator</t>
-  </si>
-  <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Offense[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Offense']/@s:id]/inc-ext:CFRStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -739,18 +609,6 @@
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/nc:ActivityIdentification/nc:IdentificationID</t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/nc:ActivityDate/nc:DateTime</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Offense[ndexia:ActivityAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Offense']/@s:id]/j:Statute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>We need to add a MTOM attachment that contains a PDF representation of the citation</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CitationServedDate/nc:Date</t>
-  </si>
-  <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CitationServedIndicator</t>
   </si>
   <si>
@@ -767,11 +625,6 @@
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/nc:ActivityDescriptionText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Person[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person
-[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/@s:id]/inc-ext:PersonFishAndWildlifeLicenseIdentification/nc:IdentificationID
-</t>
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Vehicle[ndexia:VehicleAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/@s:id]/nc:VehicleCMVIndicator</t>
@@ -787,12 +640,6 @@
     <t>The name of the organization that received delivery of the citation</t>
   </si>
   <si>
-    <t>CITATION DELIVERED TO ORGANIZATION</t>
-  </si>
-  <si>
-    <t>The name of the Citation Subject Organization</t>
-  </si>
-  <si>
     <t>Morways Moving Company</t>
   </si>
   <si>
@@ -800,18 +647,6 @@
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:CitationDeliveryRecipientAssociation/nc:EntityOrganizationReference/@s:ref]/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
-/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
-/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
-/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
@@ -831,92 +666,306 @@
 /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:ImmediateFamilyAssociation/nc:PersonParentReference/@s:ref]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStateUSPostalServiceCode</t>
   </si>
   <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>Civil Relief Act Juvenile Indicator</t>
+  </si>
+  <si>
+    <t>Civil Relief Act Other Indicator</t>
+  </si>
+  <si>
+    <t>Civil Relief Act Other Text</t>
+  </si>
+  <si>
+    <t>Civil Relief Act Indicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Charge/inc-ext:RelatedCriminalChargeIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:PersonBirthLocationAssociation/nc:LocationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>Officer ID</t>
+  </si>
+  <si>
+    <t>A unique identifier assigned to an officer</t>
+  </si>
+  <si>
+    <t>ID34567</t>
+  </si>
+  <si>
+    <t>Officer Badge No.</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:EnforcementOfficial/inc-ext:EnforcementOfficialIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Officer Agency</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:EnforcementUnit[ndexia:EnforcementUnitAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/j:EnforcementUnitNumberIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>CITATION LOCATION</t>
+  </si>
+  <si>
+    <t>The highway number/street name where the citation was issued</t>
+  </si>
+  <si>
+    <t>The municipality name where the citation was issued.</t>
+  </si>
+  <si>
+    <t>A landmark or milemarker close to where the citation was issued.</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:CitationIssuedLocationAssociation[inc-ext:CitationReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/nc:LocationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CitationServedDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>Citation Delivered to (Organization)</t>
+  </si>
+  <si>
+    <t>Citation Recipient (Organization)</t>
+  </si>
+  <si>
+    <t>The name of the Organization cited</t>
+  </si>
+  <si>
+    <t>CITATION DELIVERED TO PERSON</t>
+  </si>
+  <si>
+    <t>Person Name</t>
+  </si>
+  <si>
+    <t>The name of the person that received delivery of the citation</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:CitationDeliveryRecipientAssociation/nc:EntityPersonReference/@s:ref]/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
     <t xml:space="preserve">/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location
-[ndexia:LocationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStateUSPostalServiceCode
+[ndexia:LocationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStateUSPostalServiceCode
 </t>
   </si>
   <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:EnforcementOfficial[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/j:ActivityEnforcementOfficialAssociation/nc:PersonReference/@s:ref]/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/nc:OrganizationName</t>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=
+/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage//lexs:StructuredPayload/inc-ext:IncidentReport/nc:PersonContactInformationAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ContactInformationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/j:PersonAugmentation/nc:DriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Person[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person
+[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/@s:id]/inc-ext:PersonFishAndWildlifeLicenseIdentification/nc:IdentificationID
+</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation[lexsdigest:TelephoneNumberHomeIndicator='true']
+[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/lexsdigest:TelephoneNumberReference/@s:ref]/nc:TelephoneNumberFullID</t>
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation[lexsdigest:TelephoneNumberWorkIndicator='true']
-[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/lexsdigest:TelephoneNumberReference/@s:ref]/nc:TelephoneNumberFullID</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation[lexsdigest:TelephoneNumberHomeIndicator='true']
-[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:IncidentSubject]/lexsdigest:Person/@s:id]/lexsdigest:TelephoneNumberReference/@s:ref]/nc:TelephoneNumberFullID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DriverLicense[lexslib:SameAsDigestReference/@lexslib:ref= /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id = ../j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/j:PersonAugmentation/nc:DriverLicense/@s:id]/inc-ext:DriverLicenseCDLIndicator</t>
-  </si>
-  <si>
-    <t>Civil Relief Act Juvenile Indicator</t>
-  </si>
-  <si>
-    <t>Civil Relief Act Other Indicator</t>
-  </si>
-  <si>
-    <t>Civil Relief Act Other Text</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/inc-ext:CivilReliefActIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/inc-ext:CivilReliefActOtherIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/inc-ext:CivilReliefActOtherText</t>
-  </si>
-  <si>
-    <t>Civil Relief Act Indicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/inc-ext:CivilReliefActJuvenileIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Charge/inc-ext:RelatedCriminalChargeIndicator</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:PersonBirthLocationAssociation/nc:LocationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>Officer ID</t>
-  </si>
-  <si>
-    <t>A unique identifier assigned to an officer</t>
-  </si>
-  <si>
-    <t>ID34567</t>
-  </si>
-  <si>
-    <t>Officer Badge No.</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:EnforcementOfficial/inc-ext:EnforcementOfficialIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>Officer Agency</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:EnforcementUnit[ndexia:EnforcementUnitAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonAssignedUnitAssociation/nc:OrganizationReference/@s:ref]/j:EnforcementUnitNumberIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>CITATION LOCATION</t>
-  </si>
-  <si>
-    <t>The highway number/street name where the citation was issued</t>
-  </si>
-  <si>
-    <t>The municipality name where the citation was issued.</t>
-  </si>
-  <si>
-    <t>A landmark or milemarker close to where the citation was issued.</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:CitationIssuedLocationAssociation[inc-ext:CitationReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/nc:LocationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/lexsdigest:TelephoneNumberReference/@s:ref]/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:MeasurePointValue</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHeightMeasure/nc:LengthUnitCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:MeasurePointValue</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonWeightMeasure/nc:WeightUnitCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ConveyanceRegistrationPlateIdentification/nc:IdentificationJurisdictionFIPS10-4Code</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ItemModelYearDate</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleMakeCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleColorPrimaryCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:VehicleStyleCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/j:PersonAugmentation/nc:DriverLicense/nc:DriverLicenseIdentification/j:IdentificationJurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>INH</t>
+  </si>
+  <si>
+    <t>eCitation Element</t>
+  </si>
+  <si>
+    <t>LBR</t>
+  </si>
+  <si>
+    <t>License Plate</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/nc:ActivityDateRange/nc:StartDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>Incident Start Date/Time</t>
+  </si>
+  <si>
+    <t>Incident End Date/Time</t>
+  </si>
+  <si>
+    <t>The start date/time the incident occurred</t>
+  </si>
+  <si>
+    <t>The end date/time the incident occurred</t>
+  </si>
+  <si>
+    <t>1/1/2016:01:56</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/nc:ActivityDateRange/nc:EndDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SubjectBloodAlcoholContentNumber
+</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/j:DrivingIncidentRecordedSpeedRate/nc:MeasurePointValue</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/j:DrivingIncidentRecordedSpeedRate/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/j:DrivingIncidentLegalSpeedRate/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/j:DrivingIncidentLegalSpeedRate/nc:MeasurePointValue</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:DrivingAccidentIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:DrivingAccidentFatalityIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SeatBeltViolationIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CivilReliefActIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CivilReliefActJuvenileIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CivilReliefActOtherIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CivilReliefActOtherText</t>
+  </si>
+  <si>
+    <t>Violated Statute</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:EnforcementOfficial[nc:RoleOfPersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/j:ActivityEnforcementOfficialAssociation/nc:PersonReference/@s:ref]/j:EnforcementOfficialBadgeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Organization Driver License</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DriverLicense[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/@s:id]/inc-ext:DriverLicenseCDLIndicator</t>
+  </si>
+  <si>
+    <t>Offense Description</t>
+  </si>
+  <si>
+    <t>Charge Statute</t>
+  </si>
+  <si>
+    <t>Simple Assault 13 VSA 1023 13B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Offense'][@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/nc:ActivityDocumentAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDescriptionText
+</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/nc:ActivityDescriptionText</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityOrganization/nc:Organization[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:EntityDocumentAssociation/nc:EntityOrganizationReference/@s:ref]/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>Organization Driver License State</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Organization[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:EntityDocumentAssociation/nc:EntityOrganizationReference/@s:ref]/inc-ext:OrganizationDriverLicense/nc:DriverLicenseIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Organization[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:EntityDocumentAssociation/nc:EntityOrganizationReference/@s:ref]/inc-ext:OrganizationDriverLicense/nc:DriverLicenseIdentification/j:IdentificationJurisdictionNCICLISCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:LocationOrganizationAssociation/nc:LocationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:LocationOrganizationAssociation/nc:LocationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:LocationOrganizationAssociation/nc:LocationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Location[ndexia:LocationAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:LocationOrganizationAssociation/nc:LocationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationStateUSPostalServiceCode</t>
+  </si>
+  <si>
+    <t>Organization Phone</t>
+  </si>
+  <si>
+    <t>Organization Primary Phone Number</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation[lexsdigest:TelephoneNumberPrimaryIndicator]/lexsdigest:TelephoneNumberReference/@s:ref]/nc:TelephoneNumberFullID</t>
   </si>
 </sst>
 </file>
@@ -926,7 +975,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1019,14 +1068,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF6600"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1117,6 +1178,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1127,7 +1194,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="542">
+  <cellStyleXfs count="600">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1670,8 +1737,66 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1691,9 +1816,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1707,9 +1829,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1727,8 +1846,23 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="542">
+  <cellStyles count="600">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2008,6 +2142,35 @@
     <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2266,6 +2429,35 @@
     <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2569,11 +2761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2582,30 +2774,30 @@
     <col min="2" max="2" width="39.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="105.83203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="105.83203125" style="10" customWidth="1"/>
     <col min="6" max="6" width="57.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.1640625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" ht="42">
-      <c r="A1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" ht="18">
+      <c r="A1" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2613,1434 +2805,1587 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="14"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="18" t="s">
-        <v>81</v>
+      <c r="A3" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="14"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="70">
       <c r="A4" s="2" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="D4" s="2">
         <v>82734800</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>208</v>
+      <c r="E4" s="10" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A5" s="6" t="s">
-        <v>192</v>
+      <c r="A5" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="8">
+        <v>45</v>
+      </c>
+      <c r="D5" s="7">
         <v>42304</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="F5" s="8"/>
+      <c r="E5" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A6" s="6" t="s">
-        <v>48</v>
+      <c r="A6" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="9">
+        <v>44</v>
+      </c>
+      <c r="D6" s="8">
         <v>105</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="F6" s="9"/>
+      <c r="E6" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A7" s="6" t="s">
-        <v>193</v>
+      <c r="A7" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="D7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>243</v>
+      <c r="E7" s="11" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A8" s="6" t="s">
-        <v>194</v>
+      <c r="A8" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>181</v>
       </c>
       <c r="D8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>245</v>
+      <c r="E8" s="11" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="18" t="s">
-        <v>289</v>
+      <c r="A9" s="16" t="s">
+        <v>227</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="112" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>291</v>
+        <v>229</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>293</v>
+        <v>118</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>290</v>
+        <v>228</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>246</v>
+        <v>129</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>292</v>
+        <v>230</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>247</v>
+        <v>130</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="17" t="s">
-        <v>62</v>
+      <c r="A13" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="15"/>
+      <c r="E13" s="13"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="70">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="84">
+      <c r="A15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="84">
+      <c r="A16" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="84">
+      <c r="A17" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3">
+        <v>5401</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="84">
+      <c r="A19" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="84">
+      <c r="A20" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A21" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D21" s="3">
+        <v>8023632334</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="70">
+      <c r="A22" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="70">
+      <c r="A24" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="70">
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="70">
+      <c r="A27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="70">
+      <c r="A28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="112">
+      <c r="A29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="112">
+      <c r="A30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="140">
+      <c r="A31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="84">
+      <c r="A33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="2">
+        <v>41444812</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="84">
+      <c r="A34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="70">
+      <c r="A35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="140">
+      <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="3">
+        <v>8023631111</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="3">
+        <v>8023631112</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="7">
+        <v>24014</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A41" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="3">
+        <v>70</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A43" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="3">
+        <v>135</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="70">
-      <c r="A16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D16" s="2" t="s">
+    </row>
+    <row r="45" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A45" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E45" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" ht="70">
-      <c r="A18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="2" t="s">
+    </row>
+    <row r="46" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A46" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="70">
-      <c r="A19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="70">
-      <c r="A20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="112">
-      <c r="A21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="112">
-      <c r="A22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="140">
-      <c r="A23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="84">
-      <c r="A25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="2">
-        <v>41444812</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="84">
-      <c r="A26" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="140">
-      <c r="A27" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="2">
-        <v>12345678</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="3">
-        <v>8023631111</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="3">
-        <v>8023631112</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="8">
-        <v>24014</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A32" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A34" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="3">
-        <v>135</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A36" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A37" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A38" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A40" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A41" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A42" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A43" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="3">
-        <v>2015</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A44" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A45" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A46" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>207</v>
+      <c r="E46" s="14" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A47" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A50" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A51" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A52" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="3">
+        <v>2015</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A53" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A54" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A55" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A56" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A57" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A59" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A60" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A61" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A62" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" s="7"/>
+      <c r="E62" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" s="3" customFormat="1" ht="126">
+      <c r="A63" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A64" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A65" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A66" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A67" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A48" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A50" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A51" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="F51" s="8"/>
-    </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" ht="126">
-      <c r="A52" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A53" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C53" s="3" t="s">
+      <c r="C67" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D67" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A68" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" s="3">
         <v>30</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A54" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A55" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A56" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A57" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" s="3">
-        <v>30</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A58" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A59" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D59" s="3">
-        <v>40</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A60" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A61" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D61" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A62" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D62" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A63" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D63" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="70">
-      <c r="A64" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D64" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="70">
-      <c r="A65" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D65" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" s="12" t="s">
+      <c r="E68" s="11" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="70">
-      <c r="A66" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D66" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="70">
-      <c r="A67" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A69" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>42</v>
+        <v>175</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A70" s="6" t="s">
-        <v>112</v>
+        <v>153</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A70" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>233</v>
+        <v>34</v>
+      </c>
+      <c r="D70" s="3">
+        <v>40</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A71" s="6" t="s">
-        <v>159</v>
+      <c r="A71" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>43</v>
+        <v>176</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>232</v>
+        <v>153</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A72" s="6" t="s">
-        <v>113</v>
+      <c r="A72" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E72" s="12" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A73" s="6" t="s">
-        <v>161</v>
+        <v>35</v>
+      </c>
+      <c r="D72" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A73" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>186</v>
+        <v>65</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D73" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="E73" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="F73" s="6"/>
+      <c r="E73" s="11" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="74" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="70">
+      <c r="A75" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="70">
+      <c r="A76" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="70">
+      <c r="A77" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="70">
+      <c r="A78" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A80" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A81" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A82" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A83" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A84" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D84" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F84" s="6"/>
+    </row>
+    <row r="85" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A85" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D85" s="3">
+        <v>2</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A86" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D86" s="8">
+        <v>47</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="F86" s="8"/>
+    </row>
+    <row r="87" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A87" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D87" s="8">
+        <v>1197</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F87" s="8"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A89" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A90" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A91" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D91" s="3">
+        <v>12345</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A92" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A93" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="1:6" ht="70">
+      <c r="A95" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96" spans="1:6" ht="70">
+      <c r="A96" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D74" s="3">
-        <v>2</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A75" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D75" s="9">
-        <v>47</v>
-      </c>
-      <c r="E75" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="F75" s="9"/>
-    </row>
-    <row r="76" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A76" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D76" s="9">
-        <v>1197</v>
-      </c>
-      <c r="E76" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="F76" s="9"/>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="15"/>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A78" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E78" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A79" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A80" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="D80" s="3">
-        <v>12345</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A81" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A82" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="15"/>
-      <c r="F83" s="5"/>
-    </row>
-    <row r="84" spans="1:6" ht="70">
-      <c r="A84" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" ht="70">
-      <c r="A85" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E85" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="112">
-      <c r="A86" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E86" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="F86" s="3"/>
-    </row>
-    <row r="87" spans="1:6" ht="112">
-      <c r="A87" s="3" t="s">
+      <c r="E96" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="112">
+      <c r="A97" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="F97" s="3"/>
+    </row>
+    <row r="98" spans="1:6" ht="112">
+      <c r="A98" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B98" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C98" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D87" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="1:6" ht="126">
-      <c r="A88" s="3" t="s">
+      <c r="D98" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="1:6" ht="126">
+      <c r="A99" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="F88" s="3"/>
-    </row>
-    <row r="89" spans="1:6" ht="112">
-      <c r="A89" s="3" t="s">
+      <c r="D99" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="1:6" ht="112">
+      <c r="A100" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E89" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="F89" s="3"/>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="5"/>
-    </row>
-    <row r="91" spans="1:6" ht="84">
-      <c r="A91" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="11" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="119" customHeight="1">
-      <c r="A92" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
+      <c r="D100" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="1:6" ht="119" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated and completed "Back Of Ticket" XML sample and mapping.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="2000" windowWidth="32260" windowHeight="14200"/>
+    <workbookView xWindow="-27820" yWindow="380" windowWidth="28800" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="402">
   <si>
     <t>Description</t>
   </si>
@@ -378,9 +378,6 @@
     <t>Burlington</t>
   </si>
   <si>
-    <t>05401-1122</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -405,15 +402,6 @@
     <t>SD</t>
   </si>
   <si>
-    <t>1/1/2016:01:22</t>
-  </si>
-  <si>
-    <t>Rt. 89</t>
-  </si>
-  <si>
-    <t>MileMarker 10</t>
-  </si>
-  <si>
     <t>No vehicle registration</t>
   </si>
   <si>
@@ -432,9 +420,6 @@
     <t>VT0040100</t>
   </si>
   <si>
-    <t>Burlington, PD</t>
-  </si>
-  <si>
     <t>Jack</t>
   </si>
   <si>
@@ -474,9 +459,6 @@
     <t>Related Criminal Charge Indicator</t>
   </si>
   <si>
-    <t>VIN</t>
-  </si>
-  <si>
     <t>Speed Unit of Measure</t>
   </si>
   <si>
@@ -556,9 +538,6 @@
   </si>
   <si>
     <t>Citation Number</t>
-  </si>
-  <si>
-    <t>Citation Served Date</t>
   </si>
   <si>
     <t>Citation Served Indicator</t>
@@ -638,9 +617,6 @@
   </si>
   <si>
     <t>The name of the organization that received delivery of the citation</t>
-  </si>
-  <si>
-    <t>Morways Moving Company</t>
   </si>
   <si>
     <t>The municipality name where the incident occured.</t>
@@ -693,9 +669,6 @@
     <t>A unique identifier assigned to an officer</t>
   </si>
   <si>
-    <t>ID34567</t>
-  </si>
-  <si>
     <t>Officer Badge No.</t>
   </si>
   <si>
@@ -864,9 +837,6 @@
     <t>The end date/time the incident occurred</t>
   </si>
   <si>
-    <t>1/1/2016:01:56</t>
-  </si>
-  <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/nc:ActivityDateRange/nc:EndDate/nc:DateTime</t>
   </si>
   <si>
@@ -925,9 +895,6 @@
     <t>Charge Statute</t>
   </si>
   <si>
-    <t>Simple Assault 13 VSA 1023 13B</t>
-  </si>
-  <si>
     <t xml:space="preserve">/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Offense'][@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/nc:ActivityDocumentAssociation/nc:ActivityReference/@s:ref]/nc:ActivityDescriptionText
 </t>
   </si>
@@ -966,6 +933,315 @@
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityTelephoneNumber/lexsdigest:TelephoneNumber/nc:FullTelephoneNumber[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:EntityTelephoneNumberAssociation[lexsdigest:TelephoneNumberPrimaryIndicator]/lexsdigest:TelephoneNumberReference/@s:ref]/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>Back Of Ticket Information</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/j:CitationSubject/nc:RoleOfPersonReference/@s:ref]/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Traffic Stop Reason Code</t>
+  </si>
+  <si>
+    <t>Traffic Stop Search Category</t>
+  </si>
+  <si>
+    <t>Traffic Stop Contraband Code</t>
+  </si>
+  <si>
+    <t>Traffic Stop Outcome Code</t>
+  </si>
+  <si>
+    <t>Incident Weather Condition Code</t>
+  </si>
+  <si>
+    <t>Incident Highway Condition Code</t>
+  </si>
+  <si>
+    <t>Incident Traffic Condition Code</t>
+  </si>
+  <si>
+    <t>Incident Lighting Condition Code</t>
+  </si>
+  <si>
+    <t>Radar Device ID</t>
+  </si>
+  <si>
+    <t>Radar Before Test Date/Time</t>
+  </si>
+  <si>
+    <t>Radar Before Test Tuning Forks Pass Indicator</t>
+  </si>
+  <si>
+    <t>Radar Before Test Internal Calibration Pass Indicator</t>
+  </si>
+  <si>
+    <t>Radar Before Test Speedometer Verification Pass Indicator</t>
+  </si>
+  <si>
+    <t>Radar Before Test Display Lights Pass Indicator</t>
+  </si>
+  <si>
+    <t>Radar AfterTest Date/Time</t>
+  </si>
+  <si>
+    <t>Radar After Test Tuning Forks Pass Indicator</t>
+  </si>
+  <si>
+    <t>Radar After Test Internal Calibration Pass Indicator</t>
+  </si>
+  <si>
+    <t>Radar After Test Speedometer Verification Pass Indicator</t>
+  </si>
+  <si>
+    <t>Radar After Test Display Lights Pass Indicator</t>
+  </si>
+  <si>
+    <t>Laser Device ID</t>
+  </si>
+  <si>
+    <t>Laser Before Test Date/Time</t>
+  </si>
+  <si>
+    <t>Laser Before Test Display Lights Pass Indicator</t>
+  </si>
+  <si>
+    <t>Laser AfterTest Date/Time</t>
+  </si>
+  <si>
+    <t>Laser After Test Display Lights Pass Indicator</t>
+  </si>
+  <si>
+    <t>Radar Test</t>
+  </si>
+  <si>
+    <t>Laser Test</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/vt-ts-codes:TrafficStopReasonCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/vt-ts-codes:TrafficStopSearchCategory</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/vt-ts-codes:TrafficStopContrabandCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/vt-ts-codes:TrafficStopOutcomeCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/vt-ts-codes:IncidentWeatherConditionCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/vt-ts-codes:IncidentHighwayConditionCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/vt-ts-codes:IncidentTrafficConditionCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/vt-ts-codes:IncidentLightingConditionCode</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:MeasurementDeviceIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarBeforeTestResults/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarBeforeTestResults/inc-ext:TuningForksTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarBeforeTestResults/inc-ext:InternalCalibrationTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarBeforeTestResults/inc-ext:DisplayLightsTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarBeforeTestResults/inc-ext:SpeedometerVerificationTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarAfterTestResults/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarAfterTestResults/inc-ext:TuningForksTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarAfterTestResults/inc-ext:InternalCalibrationTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarAfterTestResults/inc-ext:SpeedometerVerificationTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:RadarDeviceTest/inc-ext:RadarAfterTestResults/inc-ext:DisplayLightsTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:MeasurementDeviceIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserBeforeTestResults/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserBeforeTestResults/inc-ext:DisplayLightsTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserAfterTestResults/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserAfterTestResults/inc-ext:DisplayLightsTestPassIndicator</t>
+  </si>
+  <si>
+    <t>Laser Before Test Scope Alignment Pass Indicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserBeforeTestResults/inc-ext:SelfTestTestPassIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserBeforeTestResults/inc-ext:ScopeAlignmentTestPassIndicator</t>
+  </si>
+  <si>
+    <t>Laser Before Test Known Distance Pass Indicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserBeforeTestResults/inc-ext:KnownDistanceTestPassIndicator</t>
+  </si>
+  <si>
+    <t>Laser Before Self Test Pass Indicator</t>
+  </si>
+  <si>
+    <t>Laser After Test Self Test Pass Indicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserAfterTestResults/inc-ext:SelfTestTestPassIndicator</t>
+  </si>
+  <si>
+    <t>Laser After Test Scope Alignment Pass Indicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserAfterTestResults/inc-ext:ScopeAlignmentTestPassIndicator</t>
+  </si>
+  <si>
+    <t>Laser After Test Known Distance Pass Indicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SpeedMeasurementDeviceTest/inc-ext:LaserDeviceTest/inc-ext:LaserAfterTestResults/inc-ext:KnownDistanceTestPassIndicator</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>SPC</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Raining</t>
+  </si>
+  <si>
+    <t>Wet</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Daylight</t>
+  </si>
+  <si>
+    <t>Radar1234</t>
+  </si>
+  <si>
+    <t>2001-12-31T12:00:00</t>
+  </si>
+  <si>
+    <t>2001-12-31T12:06:00</t>
+  </si>
+  <si>
+    <t>Laser1234</t>
+  </si>
+  <si>
+    <t>2001-12-31T12:08:00</t>
+  </si>
+  <si>
+    <t>Citation Served Date/Time</t>
+  </si>
+  <si>
+    <t>2012-08-02T10:30:04.048-04:00</t>
+  </si>
+  <si>
+    <t>105.00</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Milton</t>
+  </si>
+  <si>
+    <t>US 91</t>
+  </si>
+  <si>
+    <t>123 Allen Drive, Milton, VT, 05468</t>
+  </si>
+  <si>
+    <t>CITATION DELIVERED TO ORGANIZATION</t>
+  </si>
+  <si>
+    <t>Jones, Jennifer, J</t>
+  </si>
+  <si>
+    <t>Citation Delivered to (Person)</t>
+  </si>
+  <si>
+    <t>145 Austin Dr</t>
+  </si>
+  <si>
+    <t>806-383-1111</t>
+  </si>
+  <si>
+    <t>802-363-0046</t>
+  </si>
+  <si>
+    <t>VIN123456</t>
+  </si>
+  <si>
+    <t>2016-08-10T07:10:42</t>
+  </si>
+  <si>
+    <t>2016-08-17T20:24:41</t>
+  </si>
+  <si>
+    <t>Speeding</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>47.00</t>
+  </si>
+  <si>
+    <t>1197.00</t>
+  </si>
+  <si>
+    <t>ID467023</t>
+  </si>
+  <si>
+    <t>Burlington Police Department</t>
+  </si>
+  <si>
+    <t>802-864-3333</t>
   </si>
 </sst>
 </file>
@@ -975,7 +1251,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1086,8 +1362,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1180,7 +1462,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1194,7 +1482,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="600">
+  <cellStyleXfs count="668">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1795,8 +2083,76 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1858,11 +2214,29 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="600">
+  <cellStyles count="668">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2171,6 +2545,40 @@
     <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="627" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="629" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="631" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="633" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2458,6 +2866,40 @@
     <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="618" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="620" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="622" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="624" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="626" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="628" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="630" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="632" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="634" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="636" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="638" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="640" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="642" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="644" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="646" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="648" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="650" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="652" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="654" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="656" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="658" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="660" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="664" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="666" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2761,19 +3203,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="105.83203125" style="10" customWidth="1"/>
     <col min="6" max="6" width="57.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.1640625" style="2" customWidth="1"/>
@@ -2782,13 +3224,13 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" ht="18">
       <c r="A1" s="18" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>111</v>
@@ -2797,327 +3239,347 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="4"/>
+      <c r="A2" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="12"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="70">
-      <c r="A4" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D4" s="2">
+    <row r="3" spans="1:6" ht="70">
+      <c r="A3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="2">
         <v>82734800</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>187</v>
-      </c>
+      <c r="E3" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A4" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A5" s="3" t="s">
-        <v>179</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="7">
-        <v>42304</v>
+        <v>44</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>381</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>190</v>
+      </c>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A6" s="3" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="8">
-        <v>105</v>
+        <v>173</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>364</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="F6" s="8"/>
+        <v>189</v>
+      </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A7" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <v>1</v>
+        <v>174</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>382</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A8" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="112" customHeight="1">
+      <c r="D8" s="4"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="112" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>118</v>
+        <v>384</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>129</v>
+        <v>385</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="70">
-      <c r="A14" s="17" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="70">
+      <c r="A13" s="17" t="s">
         <v>3</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="84">
+      <c r="A14" s="20" t="s">
+        <v>51</v>
+      </c>
       <c r="B14" s="2" t="s">
-        <v>235</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>234</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="84">
       <c r="A15" s="20" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="84">
       <c r="A16" s="20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="84">
-      <c r="A17" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>112</v>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5495</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="3">
-        <v>5401</v>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="84">
+      <c r="A18" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D18" s="2">
+        <v>11846050</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="84">
       <c r="A19" s="17" t="s">
-        <v>292</v>
+        <v>289</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="84">
-      <c r="A20" s="17" t="s">
-        <v>300</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A21" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D21" s="3">
-        <v>8023632334</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>309</v>
-      </c>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A20" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="70">
       <c r="A22" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>206</v>
+        <v>143</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="15" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3127,19 +3589,19 @@
     </row>
     <row r="24" spans="1:6" ht="70">
       <c r="A24" s="2" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>233</v>
+        <v>388</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>206</v>
+        <v>387</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3166,7 +3628,7 @@
         <v>114</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="70">
@@ -3183,7 +3645,7 @@
         <v>115</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="70">
@@ -3200,7 +3662,7 @@
         <v>116</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="112">
@@ -3214,10 +3676,10 @@
         <v>15</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>117</v>
+        <v>389</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="112">
@@ -3234,7 +3696,7 @@
         <v>118</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="140">
@@ -3251,7 +3713,7 @@
         <v>112</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3264,11 +3726,11 @@
       <c r="C32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>119</v>
+      <c r="D32" s="3">
+        <v>5401</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="84">
@@ -3282,10 +3744,10 @@
         <v>10</v>
       </c>
       <c r="D33" s="2">
-        <v>41444812</v>
+        <v>1209345</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="84">
@@ -3293,7 +3755,7 @@
         <v>83</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
@@ -3302,7 +3764,7 @@
         <v>112</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="70">
@@ -3310,7 +3772,7 @@
         <v>82</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>8</v>
@@ -3319,7 +3781,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="140">
@@ -3336,7 +3798,7 @@
         <v>12345678</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3344,16 +3806,16 @@
         <v>16</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="3">
-        <v>8023631111</v>
+      <c r="D37" s="3" t="s">
+        <v>390</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3361,16 +3823,16 @@
         <v>17</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="3">
-        <v>8023631112</v>
+      <c r="D38" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3384,10 +3846,10 @@
         <v>18</v>
       </c>
       <c r="D39" s="7">
-        <v>24014</v>
+        <v>24092</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="F39" s="7"/>
     </row>
@@ -3402,27 +3864,27 @@
         <v>59</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A41" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3439,21 +3901,21 @@
         <v>70</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A43" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3470,7 +3932,7 @@
         <v>135</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3478,47 +3940,47 @@
         <v>108</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A46" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A47" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3536,16 +3998,16 @@
         <v>60</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>151</v>
+        <v>392</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3556,13 +4018,13 @@
         <v>88</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3570,7 +4032,7 @@
         <v>89</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>5</v>
@@ -3579,7 +4041,7 @@
         <v>112</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3587,7 +4049,7 @@
         <v>90</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>24</v>
@@ -3596,7 +4058,7 @@
         <v>2015</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3604,16 +4066,16 @@
         <v>91</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3621,16 +4083,16 @@
         <v>92</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3638,33 +4100,33 @@
         <v>93</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A56" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D56" s="3" t="b">
-        <v>0</v>
+      <c r="D56" s="27" t="s">
+        <v>382</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3677,11 +4139,11 @@
       <c r="C57" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="3" t="b">
-        <v>0</v>
+      <c r="D57" s="27" t="s">
+        <v>382</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3699,7 +4161,7 @@
         <v>95</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>95</v>
@@ -3708,43 +4170,43 @@
         <v>113</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A60" s="3" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>128</v>
+        <v>263</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>393</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A61" s="3" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>276</v>
+        <v>264</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>394</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="F61" s="7"/>
     </row>
@@ -3752,12 +4214,17 @@
       <c r="A62" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="B62" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="C62" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D62" s="7"/>
+      <c r="D62" s="27" t="s">
+        <v>395</v>
+      </c>
       <c r="E62" s="11" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F62" s="7"/>
     </row>
@@ -3766,16 +4233,16 @@
         <v>96</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>118</v>
+      <c r="D63" s="27" t="s">
+        <v>383</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3783,16 +4250,16 @@
         <v>97</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>129</v>
+      <c r="D64" s="27" t="s">
+        <v>384</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3805,11 +4272,11 @@
       <c r="C65" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>130</v>
+      <c r="D65" s="27" t="s">
+        <v>385</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="3" customFormat="1" ht="42">
@@ -3817,16 +4284,16 @@
         <v>99</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>131</v>
+      <c r="D66" s="27" t="s">
+        <v>127</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="3" customFormat="1" ht="98">
@@ -3834,16 +4301,16 @@
         <v>100</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="27">
         <v>0.2</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3856,25 +4323,25 @@
       <c r="C68" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="27">
         <v>30</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A69" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>153</v>
+        <v>169</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>147</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3887,25 +4354,25 @@
       <c r="C70" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D70" s="3">
+      <c r="D70" s="27">
         <v>40</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A71" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>153</v>
+        <v>170</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>147</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3918,11 +4385,11 @@
       <c r="C72" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D72" s="3" t="b">
-        <v>0</v>
+      <c r="D72" s="27" t="s">
+        <v>382</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3935,11 +4402,11 @@
       <c r="C73" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D73" s="3" t="b">
-        <v>0</v>
+      <c r="D73" s="27" t="s">
+        <v>382</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3952,16 +4419,16 @@
       <c r="C74" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D74" s="3" t="b">
-        <v>0</v>
+      <c r="D74" s="27" t="s">
+        <v>382</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="70">
       <c r="A75" s="2" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>84</v>
@@ -3969,16 +4436,16 @@
       <c r="C75" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D75" s="2" t="b">
-        <v>1</v>
+      <c r="D75" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="70">
       <c r="A76" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>85</v>
@@ -3986,16 +4453,16 @@
       <c r="C76" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D76" s="2" t="b">
-        <v>1</v>
+      <c r="D76" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="70">
       <c r="A77" s="2" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>86</v>
@@ -4003,25 +4470,25 @@
       <c r="C77" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D77" s="2" t="b">
-        <v>1</v>
+      <c r="D77" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="70">
       <c r="A78" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D78" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D78" s="26" t="s">
         <v>80</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -4035,25 +4502,25 @@
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A80" s="21" t="s">
+      <c r="A80" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A81" s="21" t="s">
-        <v>149</v>
+      <c r="A81" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>69</v>
@@ -4062,61 +4529,61 @@
         <v>40</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A82" s="21" t="s">
+      <c r="A82" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A83" s="21" t="s">
-        <v>294</v>
+      <c r="A83" s="3" t="s">
+        <v>284</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>296</v>
+        <v>396</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A84" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D84" s="3" t="b">
-        <v>0</v>
+      <c r="D84" s="27" t="s">
+        <v>382</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F84" s="6"/>
     </row>
@@ -4130,11 +4597,11 @@
       <c r="C85" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D85" s="27">
         <v>2</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="3" customFormat="1" ht="70">
@@ -4147,11 +4614,11 @@
       <c r="C86" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D86" s="8">
-        <v>47</v>
+      <c r="D86" s="27" t="s">
+        <v>397</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="F86" s="8"/>
     </row>
@@ -4165,11 +4632,11 @@
       <c r="C87" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D87" s="8">
-        <v>1197</v>
+      <c r="D87" s="27" t="s">
+        <v>398</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F87" s="8"/>
     </row>
@@ -4194,27 +4661,27 @@
         <v>46</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A90" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>222</v>
+        <v>399</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="3" customFormat="1" ht="84">
@@ -4225,30 +4692,30 @@
         <v>107</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D91" s="3">
         <v>12345</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A92" s="3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="3" customFormat="1" ht="70">
@@ -4262,10 +4729,10 @@
         <v>48</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>137</v>
+        <v>400</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -4289,10 +4756,10 @@
         <v>2</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F95" s="3"/>
     </row>
@@ -4310,7 +4777,7 @@
         <v>114</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="112">
@@ -4324,10 +4791,10 @@
         <v>51</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="F97" s="3"/>
     </row>
@@ -4342,10 +4809,10 @@
         <v>4</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F98" s="3"/>
     </row>
@@ -4363,7 +4830,7 @@
         <v>112</v>
       </c>
       <c r="E99" s="10" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F99" s="3"/>
     </row>
@@ -4378,14 +4845,384 @@
         <v>6</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="1:6" ht="119" customHeight="1"/>
+    <row r="101" spans="1:6" ht="31" customHeight="1">
+      <c r="A101" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="22"/>
+      <c r="F101" s="21"/>
+    </row>
+    <row r="102" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A102" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E102" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="70">
+      <c r="A103" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E103" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="70">
+      <c r="A104" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E104" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="70">
+      <c r="A105" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E105" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="70">
+      <c r="A106" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E106" s="11" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="70">
+      <c r="A107" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E107" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="70">
+      <c r="A108" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E108" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="70">
+      <c r="A109" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E109" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="70">
+      <c r="A110" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="14" customHeight="1">
+      <c r="A111" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="B111" s="24"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="24"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="24"/>
+    </row>
+    <row r="112" spans="1:6" ht="73" customHeight="1">
+      <c r="A112" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="84">
+      <c r="A113" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="84">
+      <c r="A114" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D114" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E114" s="11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="84">
+      <c r="A115" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D115" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="84">
+      <c r="A116" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D116" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E116" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="84">
+      <c r="A117" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D117" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E117" s="11" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="84">
+      <c r="A118" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E118" s="11" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="84">
+      <c r="A119" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D119" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E119" s="11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="84">
+      <c r="A120" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D120" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E120" s="11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="84">
+      <c r="A121" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D121" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="84">
+      <c r="A122" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D122" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="14" customHeight="1">
+      <c r="A123" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B123" s="24"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="25"/>
+      <c r="F123" s="24"/>
+    </row>
+    <row r="124" spans="1:6" ht="84">
+      <c r="A124" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E124" s="11" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="84">
+      <c r="A125" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E125" s="11" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="84">
+      <c r="A126" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D126" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E126" s="11" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="84">
+      <c r="A127" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D127" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E127" s="11" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="84">
+      <c r="A128" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D128" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E128" s="11" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="84">
+      <c r="A129" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D129" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E129" s="11" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="84">
+      <c r="A130" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E130" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="84">
+      <c r="A131" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D131" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E131" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="84">
+      <c r="A132" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D132" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E132" s="11" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="84">
+      <c r="A133" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D133" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E133" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="84">
+      <c r="A134" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D134" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E134" s="11" t="s">
+        <v>351</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated XML samples for Citation.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27820" yWindow="380" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="4760" yWindow="1040" windowWidth="28800" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="409">
   <si>
     <t>Description</t>
   </si>
@@ -1242,6 +1242,27 @@
   </si>
   <si>
     <t>802-864-3333</t>
+  </si>
+  <si>
+    <t>Model of the vehicle</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Corolla</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/nc:PersonConveyanceAssociation[nc:PersonReference/@s:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson[j:CitationSubject]/lexsdigest:Person/@s:id]/nc:ConveyanceReference/@s:ref]/nc:ItemModelName</t>
+  </si>
+  <si>
+    <t>Vehicle Model</t>
+  </si>
+  <si>
+    <t>Officer Notes</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:EnforcementOfficialNotesText</t>
   </si>
 </sst>
 </file>
@@ -1482,7 +1503,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="668">
+  <cellStyleXfs count="676">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1509,6 +1530,14 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2236,7 +2265,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="668">
+  <cellStyles count="676">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2579,6 +2608,10 @@
     <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="669" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="671" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="673" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2900,6 +2933,10 @@
     <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="664" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="666" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="668" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="670" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="672" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="674" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -3203,11 +3240,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4080,1146 +4117,1174 @@
     </row>
     <row r="54" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A54" s="3" t="s">
-        <v>92</v>
+        <v>406</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>153</v>
+        <v>402</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>26</v>
+        <v>403</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>125</v>
+        <v>404</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>255</v>
+        <v>405</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A55" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A56" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E56" s="11" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A56" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D56" s="27" t="s">
-        <v>382</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A57" s="3" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D57" s="27" t="s">
         <v>382</v>
       </c>
       <c r="E57" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A58" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="E58" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="15" t="s">
+    <row r="59" spans="1:6">
+      <c r="A59" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="5"/>
-    </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A59" s="2" t="s">
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="E60" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A60" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>393</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="F60" s="7"/>
+      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A61" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A62" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D61" s="27" t="s">
+      <c r="D62" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="E61" s="11" t="s">
+      <c r="E62" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="F61" s="7"/>
-    </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A62" s="3" t="s">
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A63" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D62" s="27" t="s">
+      <c r="D63" s="27" t="s">
         <v>395</v>
       </c>
-      <c r="E62" s="11" t="s">
+      <c r="E63" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="126">
-      <c r="A63" s="3" t="s">
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" s="3" customFormat="1" ht="126">
+      <c r="A64" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D63" s="27" t="s">
+      <c r="D64" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="E64" s="11" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A64" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>384</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A65" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A66" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D65" s="27" t="s">
+      <c r="D66" s="27" t="s">
         <v>385</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="E66" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A66" s="3" t="s">
+    <row r="67" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A67" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D66" s="27" t="s">
+      <c r="D67" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="E67" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A67" s="3" t="s">
+    <row r="68" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A68" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D67" s="27">
+      <c r="D68" s="27">
         <v>0.2</v>
       </c>
-      <c r="E67" s="11" t="s">
+      <c r="E68" s="11" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A68" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D68" s="27">
-        <v>30</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A69" s="3" t="s">
-        <v>146</v>
+        <v>33</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D69" s="27" t="s">
-        <v>147</v>
+        <v>62</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" s="27">
+        <v>30</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A70" s="3" t="s">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D70" s="27">
-        <v>40</v>
+        <v>169</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>147</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A71" s="3" t="s">
-        <v>146</v>
+        <v>34</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D71" s="27" t="s">
-        <v>147</v>
+        <v>63</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="27">
+        <v>40</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A72" s="3" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>35</v>
+        <v>170</v>
       </c>
       <c r="D72" s="27" t="s">
-        <v>382</v>
+        <v>147</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A73" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D73" s="27" t="s">
         <v>382</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A74" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D74" s="27" t="s">
         <v>382</v>
       </c>
       <c r="E74" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A75" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="E75" s="11" t="s">
         <v>275</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="70">
-      <c r="A75" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D75" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="70">
       <c r="A76" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D76" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="70">
       <c r="A77" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D77" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="70">
       <c r="A78" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D78" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="70">
+      <c r="A79" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D78" s="26" t="s">
+      <c r="D79" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="E79" s="11" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="15" t="s">
+    <row r="80" spans="1:6">
+      <c r="A80" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="5"/>
-    </row>
-    <row r="80" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A80" s="3" t="s">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A81" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C81" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D81" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E80" s="11" t="s">
+      <c r="E81" s="11" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A81" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E81" s="11" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A82" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A83" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D83" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E82" s="11" t="s">
+      <c r="E83" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A83" s="3" t="s">
+    <row r="84" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A84" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="E84" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A84" s="3" t="s">
+    <row r="85" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A85" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D84" s="27" t="s">
+      <c r="D85" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="E84" s="11" t="s">
+      <c r="E85" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="F84" s="6"/>
-    </row>
-    <row r="85" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A85" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D85" s="27">
-        <v>2</v>
-      </c>
-      <c r="E85" s="11" t="s">
-        <v>185</v>
-      </c>
+      <c r="F85" s="6"/>
     </row>
     <row r="86" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A86" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D86" s="27" t="s">
-        <v>397</v>
+        <v>41</v>
+      </c>
+      <c r="D86" s="27">
+        <v>2</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F86" s="8"/>
+        <v>185</v>
+      </c>
     </row>
     <row r="87" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A87" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F87" s="8"/>
+    </row>
+    <row r="88" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A88" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D87" s="27" t="s">
+      <c r="D88" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="E88" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="F87" s="8"/>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="15" t="s">
+      <c r="F88" s="8"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="5"/>
-    </row>
-    <row r="89" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A89" s="3" t="s">
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A90" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D90" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E89" s="11" t="s">
+      <c r="E90" s="11" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A90" s="3" t="s">
+    <row r="91" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A91" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D91" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="E90" s="11" t="s">
+      <c r="E91" s="11" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A91" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="D91" s="3">
-        <v>12345</v>
-      </c>
-      <c r="E91" s="11" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A92" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D92" s="3">
+        <v>12345</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A93" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C93" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D93" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="E93" s="11" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A93" s="3" t="s">
+    <row r="94" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A94" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B94" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D94" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="E93" s="11" t="s">
+      <c r="E94" s="11" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="15" t="s">
+    <row r="95" spans="1:6">
+      <c r="A95" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="5"/>
-    </row>
-    <row r="95" spans="1:6" ht="70">
-      <c r="A95" s="3" t="s">
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6" ht="70">
+      <c r="A96" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E95" s="10" t="s">
+      <c r="E96" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="F95" s="3"/>
-    </row>
-    <row r="96" spans="1:6" ht="70">
-      <c r="A96" s="2" t="s">
+      <c r="F96" s="3"/>
+    </row>
+    <row r="97" spans="1:6" ht="70">
+      <c r="A97" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E96" s="10" t="s">
+      <c r="E97" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="112">
-      <c r="A97" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="F97" s="3"/>
     </row>
     <row r="98" spans="1:6" ht="112">
       <c r="A98" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="1:6" ht="112">
+      <c r="A99" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D99" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E98" s="10" t="s">
+      <c r="E99" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="F98" s="3"/>
-    </row>
-    <row r="99" spans="1:6" ht="126">
-      <c r="A99" s="3" t="s">
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="1:6" ht="126">
+      <c r="A100" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D100" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E99" s="10" t="s">
+      <c r="E100" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="F99" s="3"/>
-    </row>
-    <row r="100" spans="1:6" ht="112">
-      <c r="A100" s="3" t="s">
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="1:6" ht="112">
+      <c r="A101" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C101" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D101" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E100" s="10" t="s">
+      <c r="E101" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="F100" s="3"/>
-    </row>
-    <row r="101" spans="1:6" ht="31" customHeight="1">
-      <c r="A101" s="23" t="s">
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:6" ht="31" customHeight="1">
+      <c r="A102" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="B101" s="21"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="21"/>
-      <c r="E101" s="22"/>
-      <c r="F101" s="21"/>
-    </row>
-    <row r="102" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A102" s="3" t="s">
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="21"/>
+      <c r="E102" s="22"/>
+      <c r="F102" s="21"/>
+    </row>
+    <row r="103" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A103" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="D103" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E102" s="14" t="s">
+      <c r="E103" s="14" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="70">
-      <c r="A103" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="E103" s="11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="70">
-      <c r="A104" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>367</v>
+    <row r="104" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A104" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>407</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>329</v>
+        <v>408</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="70">
       <c r="A105" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="70">
       <c r="A106" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="70">
       <c r="A107" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="70">
       <c r="A108" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="70">
       <c r="A109" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E109" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="70">
       <c r="A110" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="70">
+      <c r="A111" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E111" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="70">
+      <c r="A112" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D110" s="2" t="s">
+      <c r="D112" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E110" s="11" t="s">
+      <c r="E112" s="11" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="14" customHeight="1">
-      <c r="A111" s="24" t="s">
+    <row r="113" spans="1:6" ht="14" customHeight="1">
+      <c r="A113" s="24" t="s">
         <v>326</v>
       </c>
-      <c r="B111" s="24"/>
-      <c r="C111" s="24"/>
-      <c r="D111" s="24"/>
-      <c r="E111" s="25"/>
-      <c r="F111" s="24"/>
-    </row>
-    <row r="112" spans="1:6" ht="73" customHeight="1">
-      <c r="A112" s="2" t="s">
+      <c r="B113" s="24"/>
+      <c r="C113" s="24"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="25"/>
+      <c r="F113" s="24"/>
+    </row>
+    <row r="114" spans="1:6" ht="73" customHeight="1">
+      <c r="A114" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D114" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="E114" s="11" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="84">
-      <c r="A113" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="E113" s="11" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="84">
-      <c r="A114" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D114" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E114" s="11" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="84">
       <c r="A115" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D115" s="26" t="s">
-        <v>364</v>
+        <v>311</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="E115" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="84">
       <c r="A116" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D116" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E116" s="11" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="84">
       <c r="A117" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D117" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="84">
       <c r="A118" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>376</v>
+        <v>314</v>
+      </c>
+      <c r="D118" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="84">
       <c r="A119" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D119" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="84">
       <c r="A120" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D120" s="26" t="s">
-        <v>364</v>
+        <v>316</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="84">
       <c r="A121" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D121" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="84">
       <c r="A122" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D122" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="14" customHeight="1">
-      <c r="A123" s="24" t="s">
-        <v>327</v>
-      </c>
-      <c r="B123" s="24"/>
-      <c r="C123" s="24"/>
-      <c r="D123" s="24"/>
-      <c r="E123" s="25"/>
-      <c r="F123" s="24"/>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="84">
+      <c r="A123" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D123" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E123" s="11" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="124" spans="1:6" ht="84">
       <c r="A124" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>377</v>
+        <v>320</v>
+      </c>
+      <c r="D124" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="84">
-      <c r="A125" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="E125" s="11" t="s">
-        <v>348</v>
-      </c>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="14" customHeight="1">
+      <c r="A125" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B125" s="24"/>
+      <c r="C125" s="24"/>
+      <c r="D125" s="24"/>
+      <c r="E125" s="25"/>
+      <c r="F125" s="24"/>
     </row>
     <row r="126" spans="1:6" ht="84">
       <c r="A126" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="D126" s="26" t="s">
-        <v>364</v>
+        <v>321</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="84">
       <c r="A127" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="D127" s="26" t="s">
-        <v>364</v>
+        <v>322</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="E127" s="11" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="84">
       <c r="A128" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D128" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="84">
       <c r="A129" s="2" t="s">
-        <v>323</v>
+        <v>352</v>
       </c>
       <c r="D129" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="84">
       <c r="A130" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>378</v>
+        <v>355</v>
+      </c>
+      <c r="D130" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="84">
       <c r="A131" s="2" t="s">
-        <v>358</v>
+        <v>323</v>
       </c>
       <c r="D131" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="84">
       <c r="A132" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="D132" s="26" t="s">
-        <v>364</v>
+        <v>324</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>378</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="84">
       <c r="A133" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D133" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="84">
       <c r="A134" s="2" t="s">
-        <v>325</v>
+        <v>360</v>
       </c>
       <c r="D134" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E134" s="11" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="84">
+      <c r="A135" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D135" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E135" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="84">
+      <c r="A136" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D136" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E136" s="11" t="s">
         <v>351</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hawaii Court filing Updates.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="1040" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="2060" yWindow="3280" windowWidth="28800" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="417">
   <si>
     <t>Description</t>
   </si>
@@ -1263,6 +1263,30 @@
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:EnforcementOfficialNotesText</t>
+  </si>
+  <si>
+    <t>Count of seat belt violation</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>Seat Belt Violation Count</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SeatBeltViolationCount</t>
+  </si>
+  <si>
+    <t>Citation Violation Date</t>
+  </si>
+  <si>
+    <t>The date of the violation</t>
+  </si>
+  <si>
+    <t>Violation Date</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CitationViolationDate/nc:DateTime</t>
   </si>
 </sst>
 </file>
@@ -1503,7 +1527,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="676">
+  <cellStyleXfs count="684">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1530,6 +1554,14 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2265,7 +2297,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="676">
+  <cellStyles count="684">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2612,6 +2644,10 @@
     <cellStyle name="Followed Hyperlink" xfId="671" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="673" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="677" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="679" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2937,6 +2973,10 @@
     <cellStyle name="Hyperlink" xfId="670" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="672" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="674" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="676" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="678" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -3240,11 +3280,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3328,1963 +3368,1996 @@
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>413</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>159</v>
+        <v>414</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>381</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="D5" s="7"/>
       <c r="E5" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="F5" s="8"/>
+        <v>416</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A6" s="3" t="s">
-        <v>173</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>173</v>
+        <v>44</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>364</v>
+        <v>381</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>189</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A7" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A8" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D8" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="16" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" ht="112" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="112" customHeight="1">
+      <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>222</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="15" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="70">
-      <c r="A13" s="17" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="70">
+      <c r="A14" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="84">
-      <c r="A14" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="84">
       <c r="A15" s="20" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="84">
       <c r="A16" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="84">
+      <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A17" s="6" t="s">
+    <row r="18" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D18" s="3">
         <v>5495</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="84">
-      <c r="A18" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D18" s="2">
-        <v>11846050</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="84">
       <c r="A19" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D19" s="2">
+        <v>11846050</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="84">
+      <c r="A20" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A20" s="6" t="s">
+    <row r="21" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A21" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="15" t="s">
+    <row r="22" spans="1:6">
+      <c r="A22" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" ht="70">
-      <c r="A22" s="20" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="70">
+      <c r="A23" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E23" s="10" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="15" t="s">
+    <row r="24" spans="1:6">
+      <c r="A24" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" ht="70">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="70">
+      <c r="A25" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="15" t="s">
+    <row r="26" spans="1:6">
+      <c r="A26" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" ht="70">
-      <c r="A26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>231</v>
-      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="70">
       <c r="A27" s="2" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="70">
       <c r="A28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="70">
+      <c r="A29" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E29" s="14" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="112">
-      <c r="A29" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="112">
       <c r="A30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="112">
+      <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="140">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:6" ht="140">
+      <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D33" s="3">
         <v>5401</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E33" s="11" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="84">
-      <c r="A33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1209345</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="84">
       <c r="A34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1209345</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="84">
+      <c r="A35" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E35" s="14" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="70">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:6" ht="70">
+      <c r="A36" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="2" t="b">
+      <c r="D36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E36" s="10" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="140">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:6" ht="140">
+      <c r="A37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D37" s="2">
         <v>12345678</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E37" s="14" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A37" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="112">
       <c r="A38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E39" s="11" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="7">
-        <v>24092</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="7">
+        <v>24092</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E41" s="14" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A42" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E42" s="11" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="3">
-        <v>70</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A43" s="3" t="s">
-        <v>142</v>
+        <v>20</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>258</v>
+        <v>20</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="3">
+        <v>70</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A44" s="3" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="3">
-        <v>135</v>
+        <v>148</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A45" s="3" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>260</v>
+        <v>21</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="3">
+        <v>135</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A46" s="3" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>22</v>
+        <v>149</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>121</v>
+        <v>260</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A47" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>121</v>
       </c>
       <c r="E47" s="14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A48" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E48" s="14" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="15" t="s">
+    <row r="49" spans="1:6">
+      <c r="A49" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A49" s="3" t="s">
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A50" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A50" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="112">
       <c r="A51" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A52" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E52" s="11" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A52" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" s="3">
-        <v>2015</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A53" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>124</v>
+        <v>24</v>
+      </c>
+      <c r="D53" s="3">
+        <v>2015</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A54" s="3" t="s">
-        <v>406</v>
+        <v>91</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>402</v>
+        <v>152</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>403</v>
+        <v>25</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>404</v>
+        <v>124</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>405</v>
+        <v>254</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A55" s="3" t="s">
-        <v>92</v>
+        <v>406</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>153</v>
+        <v>402</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>26</v>
+        <v>403</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>125</v>
+        <v>404</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>255</v>
+        <v>405</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A57" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="E57" s="11" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A57" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>382</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A58" s="3" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D58" s="27" t="s">
         <v>382</v>
       </c>
       <c r="E58" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A59" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="E59" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="15" t="s">
+    <row r="60" spans="1:6">
+      <c r="A60" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="5"/>
-    </row>
-    <row r="60" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A60" s="2" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A61" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E60" s="11" t="s">
+      <c r="E61" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A61" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D61" s="27" t="s">
-        <v>393</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="F61" s="7"/>
+      <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A62" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A63" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D62" s="27" t="s">
+      <c r="D63" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="E62" s="11" t="s">
+      <c r="E63" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A63" s="3" t="s">
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A64" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D63" s="27" t="s">
+      <c r="D64" s="27" t="s">
         <v>395</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="E64" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="F63" s="7"/>
-    </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" ht="126">
-      <c r="A64" s="3" t="s">
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:5" s="3" customFormat="1" ht="126">
+      <c r="A65" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="27" t="s">
+      <c r="D65" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="E65" s="11" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A65" s="3" t="s">
+    <row r="66" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="A66" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D65" s="27" t="s">
+      <c r="D66" s="27" t="s">
         <v>384</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="E66" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A66" s="3" t="s">
+    <row r="67" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="A67" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D66" s="27" t="s">
+      <c r="D67" s="27" t="s">
         <v>385</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="E67" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A67" s="3" t="s">
+    <row r="68" spans="1:5" s="3" customFormat="1" ht="42">
+      <c r="A68" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D67" s="27" t="s">
+      <c r="D68" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="E67" s="11" t="s">
+      <c r="E68" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A68" s="3" t="s">
+    <row r="69" spans="1:5" s="3" customFormat="1" ht="98">
+      <c r="A69" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D68" s="27">
+      <c r="D69" s="27">
         <v>0.2</v>
       </c>
-      <c r="E68" s="11" t="s">
+      <c r="E69" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A69" s="3" t="s">
+    <row r="70" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="A70" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D69" s="27">
+      <c r="D70" s="27">
         <v>30</v>
       </c>
-      <c r="E69" s="11" t="s">
+      <c r="E70" s="11" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A70" s="3" t="s">
+    <row r="71" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="A71" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D70" s="27" t="s">
+      <c r="D71" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="E71" s="11" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A71" s="3" t="s">
+    <row r="72" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="A72" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D71" s="27">
+      <c r="D72" s="27">
         <v>40</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="E72" s="11" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A72" s="3" t="s">
+    <row r="73" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="A73" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D72" s="27" t="s">
+      <c r="D73" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="E72" s="11" t="s">
+      <c r="E73" s="11" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A73" s="3" t="s">
+    <row r="74" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="A74" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D73" s="27" t="s">
-        <v>382</v>
-      </c>
-      <c r="E73" s="11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A74" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="D74" s="27" t="s">
         <v>382</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="3" customFormat="1" ht="70">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A75" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D75" s="27" t="s">
         <v>382</v>
       </c>
       <c r="E75" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="A76" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="E76" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="70">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:5" s="3" customFormat="1" ht="70">
+      <c r="A77" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="70">
+      <c r="A78" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D76" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="70">
-      <c r="A77" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D77" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="70">
-      <c r="A78" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D78" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E78" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="70">
+      <c r="A79" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D79" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="70">
+      <c r="A80" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="70">
-      <c r="A79" s="2" t="s">
+    <row r="81" spans="1:6" ht="70">
+      <c r="A81" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D79" s="26" t="s">
+      <c r="D81" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="E79" s="11" t="s">
+      <c r="E81" s="11" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="15" t="s">
+    <row r="82" spans="1:6">
+      <c r="A82" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="5"/>
-    </row>
-    <row r="81" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A81" s="3" t="s">
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A83" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D83" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E81" s="11" t="s">
+      <c r="E83" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A82" s="3" t="s">
+    <row r="84" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A84" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E82" s="11" t="s">
+      <c r="E84" s="11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A83" s="3" t="s">
+    <row r="85" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A85" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D85" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="E85" s="11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A84" s="3" t="s">
+    <row r="86" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A86" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B86" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D86" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="E84" s="11" t="s">
+      <c r="E86" s="11" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A85" s="3" t="s">
+    <row r="87" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A87" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D85" s="27" t="s">
+      <c r="D87" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="E85" s="11" t="s">
+      <c r="E87" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="F85" s="6"/>
-    </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A86" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D86" s="27">
-        <v>2</v>
-      </c>
-      <c r="E86" s="11" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A87" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D87" s="27" t="s">
-        <v>397</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F87" s="8"/>
+      <c r="F87" s="6"/>
     </row>
     <row r="88" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A88" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D88" s="27" t="s">
-        <v>398</v>
+        <v>41</v>
+      </c>
+      <c r="D88" s="27">
+        <v>2</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="F88" s="8"/>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="13"/>
-      <c r="F89" s="5"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A89" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D89" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F89" s="8"/>
     </row>
     <row r="90" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A90" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D90" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F90" s="8"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A92" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C92" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D92" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E90" s="11" t="s">
+      <c r="E92" s="11" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A91" s="3" t="s">
+    <row r="93" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A93" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C93" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D93" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="E91" s="11" t="s">
+      <c r="E93" s="11" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A92" s="3" t="s">
+    <row r="94" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A94" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B94" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D92" s="3">
+      <c r="D94" s="3">
         <v>12345</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="E94" s="11" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A93" s="3" t="s">
+    <row r="95" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A95" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B95" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D95" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E93" s="11" t="s">
+      <c r="E95" s="11" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A94" s="3" t="s">
+    <row r="96" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A96" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="E94" s="11" t="s">
+      <c r="E96" s="11" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="15" t="s">
+    <row r="97" spans="1:6">
+      <c r="A97" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="13"/>
-      <c r="F95" s="5"/>
-    </row>
-    <row r="96" spans="1:6" ht="70">
-      <c r="A96" s="3" t="s">
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="1:6" ht="70">
+      <c r="A98" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B98" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C98" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D98" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E96" s="10" t="s">
+      <c r="E98" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="F96" s="3"/>
-    </row>
-    <row r="97" spans="1:6" ht="70">
-      <c r="A97" s="2" t="s">
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="1:6" ht="70">
+      <c r="A99" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B99" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E97" s="10" t="s">
+      <c r="E99" s="10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="112">
-      <c r="A98" s="3" t="s">
+    <row r="100" spans="1:6" ht="112">
+      <c r="A100" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D100" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E98" s="10" t="s">
+      <c r="E100" s="10" t="s">
         <v>201</v>
-      </c>
-      <c r="F98" s="3"/>
-    </row>
-    <row r="99" spans="1:6" ht="112">
-      <c r="A99" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E99" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="F99" s="3"/>
-    </row>
-    <row r="100" spans="1:6" ht="126">
-      <c r="A100" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E100" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="F100" s="3"/>
     </row>
     <row r="101" spans="1:6" ht="112">
       <c r="A101" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:6" ht="126">
+      <c r="A102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="1:6" ht="112">
+      <c r="A103" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C103" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D103" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E101" s="10" t="s">
+      <c r="E103" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="F101" s="3"/>
-    </row>
-    <row r="102" spans="1:6" ht="31" customHeight="1">
-      <c r="A102" s="23" t="s">
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="1:6" ht="31" customHeight="1">
+      <c r="A104" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="B102" s="21"/>
-      <c r="C102" s="21"/>
-      <c r="D102" s="21"/>
-      <c r="E102" s="22"/>
-      <c r="F102" s="21"/>
-    </row>
-    <row r="103" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A103" s="3" t="s">
+      <c r="B104" s="21"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="21"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="21"/>
+    </row>
+    <row r="105" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A105" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E103" s="14" t="s">
+      <c r="E105" s="14" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A104" s="3" t="s">
+    <row r="106" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A106" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D106" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="E104" s="11" t="s">
+      <c r="E106" s="11" t="s">
         <v>408</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="70">
-      <c r="A105" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="E105" s="11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="70">
-      <c r="A106" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="E106" s="11" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="70">
       <c r="A107" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="70">
       <c r="A108" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="70">
       <c r="A109" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E109" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="70">
       <c r="A110" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="70">
       <c r="A111" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="70">
       <c r="A112" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="70">
+      <c r="A113" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="70">
+      <c r="A114" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D114" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="E114" s="11" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="14" customHeight="1">
-      <c r="A113" s="24" t="s">
+    <row r="115" spans="1:6" ht="14" customHeight="1">
+      <c r="A115" s="24" t="s">
         <v>326</v>
       </c>
-      <c r="B113" s="24"/>
-      <c r="C113" s="24"/>
-      <c r="D113" s="24"/>
-      <c r="E113" s="25"/>
-      <c r="F113" s="24"/>
-    </row>
-    <row r="114" spans="1:6" ht="73" customHeight="1">
-      <c r="A114" s="2" t="s">
+      <c r="B115" s="24"/>
+      <c r="C115" s="24"/>
+      <c r="D115" s="24"/>
+      <c r="E115" s="25"/>
+      <c r="F115" s="24"/>
+    </row>
+    <row r="116" spans="1:6" ht="73" customHeight="1">
+      <c r="A116" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D116" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E114" s="11" t="s">
+      <c r="E116" s="11" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="84">
-      <c r="A115" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="E115" s="11" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="84">
-      <c r="A116" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D116" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E116" s="11" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="84">
       <c r="A117" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D117" s="26" t="s">
-        <v>364</v>
+        <v>311</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="84">
       <c r="A118" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D118" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="84">
       <c r="A119" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D119" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="84">
       <c r="A120" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>376</v>
+        <v>314</v>
+      </c>
+      <c r="D120" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="84">
       <c r="A121" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D121" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="84">
       <c r="A122" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D122" s="26" t="s">
-        <v>364</v>
+        <v>316</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="84">
       <c r="A123" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D123" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="84">
       <c r="A124" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D124" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="14" customHeight="1">
-      <c r="A125" s="24" t="s">
-        <v>327</v>
-      </c>
-      <c r="B125" s="24"/>
-      <c r="C125" s="24"/>
-      <c r="D125" s="24"/>
-      <c r="E125" s="25"/>
-      <c r="F125" s="24"/>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="84">
+      <c r="A125" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D125" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E125" s="11" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="126" spans="1:6" ht="84">
       <c r="A126" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>377</v>
+        <v>320</v>
+      </c>
+      <c r="D126" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="84">
-      <c r="A127" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="E127" s="11" t="s">
-        <v>348</v>
-      </c>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="14" customHeight="1">
+      <c r="A127" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B127" s="24"/>
+      <c r="C127" s="24"/>
+      <c r="D127" s="24"/>
+      <c r="E127" s="25"/>
+      <c r="F127" s="24"/>
     </row>
     <row r="128" spans="1:6" ht="84">
       <c r="A128" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="D128" s="26" t="s">
-        <v>364</v>
+        <v>321</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="84">
       <c r="A129" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="D129" s="26" t="s">
-        <v>364</v>
+        <v>322</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="84">
       <c r="A130" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D130" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="84">
       <c r="A131" s="2" t="s">
-        <v>323</v>
+        <v>352</v>
       </c>
       <c r="D131" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="84">
       <c r="A132" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>378</v>
+        <v>355</v>
+      </c>
+      <c r="D132" s="26" t="s">
+        <v>364</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="84">
       <c r="A133" s="2" t="s">
-        <v>358</v>
+        <v>323</v>
       </c>
       <c r="D133" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="84">
       <c r="A134" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="D134" s="26" t="s">
-        <v>364</v>
+        <v>324</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>378</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="84">
       <c r="A135" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D135" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="84">
       <c r="A136" s="2" t="s">
-        <v>325</v>
+        <v>360</v>
       </c>
       <c r="D136" s="26" t="s">
         <v>364</v>
       </c>
       <c r="E136" s="11" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="84">
+      <c r="A137" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D137" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E137" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="84">
+      <c r="A138" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D138" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="E138" s="11" t="s">
         <v>351</v>
       </c>
     </row>

</xml_diff>

<commit_message>
XML file and xslt updates for Hawaii Court Filing
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="3280" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="5860" yWindow="3200" windowWidth="28800" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -405,9 +405,6 @@
     <t>No vehicle registration</t>
   </si>
   <si>
-    <t>20-124</t>
-  </si>
-  <si>
     <t>23CFR655</t>
   </si>
   <si>
@@ -1287,6 +1284,9 @@
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Citation[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:CitationViolationDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>SL2</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1527,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="684">
+  <cellStyleXfs count="686">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1554,6 +1554,8 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2297,7 +2299,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="684">
+  <cellStyles count="686">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2648,6 +2650,7 @@
     <cellStyle name="Followed Hyperlink" xfId="679" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2977,6 +2980,7 @@
     <cellStyle name="Hyperlink" xfId="678" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -3283,8 +3287,8 @@
   <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3301,13 +3305,13 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" ht="18">
       <c r="A1" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>111</v>
@@ -3316,7 +3320,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3333,52 +3337,52 @@
     </row>
     <row r="3" spans="1:6" ht="70">
       <c r="A3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" s="2">
         <v>82734800</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A4" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A5" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>415</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -3387,56 +3391,56 @@
         <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A7" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A8" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -3451,16 +3455,16 @@
         <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3468,16 +3472,16 @@
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3485,16 +3489,16 @@
         <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3512,16 +3516,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="84">
@@ -3538,7 +3542,7 @@
         <v>117</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="84">
@@ -3555,7 +3559,7 @@
         <v>118</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="84">
@@ -3572,7 +3576,7 @@
         <v>112</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" ht="84">
@@ -3589,63 +3593,63 @@
         <v>5495</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="84">
       <c r="A19" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D19" s="2">
         <v>11846050</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="84">
       <c r="A20" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A21" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>297</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -3658,21 +3662,21 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -3682,19 +3686,19 @@
     </row>
     <row r="25" spans="1:6" ht="70">
       <c r="A25" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3721,7 +3725,7 @@
         <v>114</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="70">
@@ -3738,7 +3742,7 @@
         <v>115</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="70">
@@ -3755,7 +3759,7 @@
         <v>116</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="112">
@@ -3769,10 +3773,10 @@
         <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="112">
@@ -3789,7 +3793,7 @@
         <v>118</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="140">
@@ -3806,7 +3810,7 @@
         <v>112</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3823,7 +3827,7 @@
         <v>5401</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="84">
@@ -3840,7 +3844,7 @@
         <v>1209345</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="84">
@@ -3848,7 +3852,7 @@
         <v>83</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>9</v>
@@ -3857,7 +3861,7 @@
         <v>112</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="70">
@@ -3865,7 +3869,7 @@
         <v>82</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>8</v>
@@ -3874,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="140">
@@ -3891,7 +3895,7 @@
         <v>12345678</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3899,16 +3903,16 @@
         <v>16</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3916,16 +3920,16 @@
         <v>17</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3942,7 +3946,7 @@
         <v>24092</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F40" s="7"/>
     </row>
@@ -3960,15 +3964,15 @@
         <v>119</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A42" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>19</v>
@@ -3977,7 +3981,7 @@
         <v>120</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3994,21 +3998,21 @@
         <v>70</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A44" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="3" customFormat="1" ht="70">
@@ -4025,7 +4029,7 @@
         <v>135</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="3" customFormat="1" ht="70">
@@ -4033,21 +4037,21 @@
         <v>108</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A47" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>22</v>
@@ -4056,15 +4060,15 @@
         <v>121</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A48" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>23</v>
@@ -4073,7 +4077,7 @@
         <v>121</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -4097,10 +4101,10 @@
         <v>60</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="112">
@@ -4111,13 +4115,13 @@
         <v>88</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="3" customFormat="1" ht="112">
@@ -4125,7 +4129,7 @@
         <v>89</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>5</v>
@@ -4134,7 +4138,7 @@
         <v>112</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="3" customFormat="1" ht="98">
@@ -4142,7 +4146,7 @@
         <v>90</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>24</v>
@@ -4151,7 +4155,7 @@
         <v>2015</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="3" customFormat="1" ht="98">
@@ -4159,7 +4163,7 @@
         <v>91</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>25</v>
@@ -4168,24 +4172,24 @@
         <v>124</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A55" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="E55" s="11" t="s">
         <v>404</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="3" customFormat="1" ht="98">
@@ -4193,7 +4197,7 @@
         <v>92</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>26</v>
@@ -4202,7 +4206,7 @@
         <v>125</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="98">
@@ -4210,7 +4214,7 @@
         <v>93</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>27</v>
@@ -4219,24 +4223,24 @@
         <v>126</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A58" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="3" customFormat="1" ht="70">
@@ -4250,10 +4254,10 @@
         <v>39</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -4271,7 +4275,7 @@
         <v>95</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>95</v>
@@ -4280,43 +4284,43 @@
         <v>113</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A62" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A63" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="E63" s="11" t="s">
         <v>266</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D63" s="27" t="s">
-        <v>394</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>267</v>
       </c>
       <c r="F63" s="7"/>
     </row>
@@ -4331,10 +4335,10 @@
         <v>99</v>
       </c>
       <c r="D64" s="27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F64" s="7"/>
     </row>
@@ -4343,16 +4347,16 @@
         <v>96</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="3" customFormat="1" ht="70">
@@ -4360,16 +4364,16 @@
         <v>97</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D66" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="3" customFormat="1" ht="70">
@@ -4383,10 +4387,10 @@
         <v>30</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="3" customFormat="1" ht="42">
@@ -4394,7 +4398,7 @@
         <v>99</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>31</v>
@@ -4403,7 +4407,7 @@
         <v>127</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="3" customFormat="1" ht="98">
@@ -4411,7 +4415,7 @@
         <v>100</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>32</v>
@@ -4420,7 +4424,7 @@
         <v>0.2</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="3" customFormat="1" ht="70">
@@ -4437,21 +4441,21 @@
         <v>30</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A71" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D71" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D71" s="27" t="s">
-        <v>147</v>
-      </c>
       <c r="E71" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="3" customFormat="1" ht="70">
@@ -4468,21 +4472,21 @@
         <v>40</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A73" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D73" s="27" t="s">
-        <v>147</v>
-      </c>
       <c r="E73" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="3" customFormat="1" ht="70">
@@ -4496,10 +4500,10 @@
         <v>35</v>
       </c>
       <c r="D74" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="3" customFormat="1" ht="70">
@@ -4513,10 +4517,10 @@
         <v>36</v>
       </c>
       <c r="D75" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="3" customFormat="1" ht="70">
@@ -4530,32 +4534,32 @@
         <v>37</v>
       </c>
       <c r="D76" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A77" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>409</v>
+      </c>
+      <c r="E77" s="11" t="s">
         <v>411</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="D77" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="70">
       <c r="A78" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>84</v>
@@ -4564,15 +4568,15 @@
         <v>52</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="70">
       <c r="A79" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>85</v>
@@ -4581,15 +4585,15 @@
         <v>53</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="70">
       <c r="A80" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>86</v>
@@ -4598,24 +4602,24 @@
         <v>54</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="70">
       <c r="A81" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D81" s="26" t="s">
         <v>80</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -4636,18 +4640,18 @@
         <v>68</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A84" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>69</v>
@@ -4656,10 +4660,10 @@
         <v>40</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="3" customFormat="1" ht="70">
@@ -4670,47 +4674,47 @@
         <v>70</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>130</v>
+        <v>416</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A86" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A87" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D87" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F87" s="6"/>
     </row>
@@ -4728,7 +4732,7 @@
         <v>2</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="3" customFormat="1" ht="70">
@@ -4742,10 +4746,10 @@
         <v>42</v>
       </c>
       <c r="D89" s="27" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F89" s="8"/>
     </row>
@@ -4760,10 +4764,10 @@
         <v>43</v>
       </c>
       <c r="D90" s="27" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F90" s="8"/>
     </row>
@@ -4788,27 +4792,27 @@
         <v>46</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="93" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A93" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B93" s="3" t="s">
-        <v>213</v>
-      </c>
       <c r="C93" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="94" spans="1:6" s="3" customFormat="1" ht="84">
@@ -4819,30 +4823,30 @@
         <v>107</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D94" s="3">
         <v>12345</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A95" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="3" customFormat="1" ht="70">
@@ -4856,10 +4860,10 @@
         <v>48</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -4883,10 +4887,10 @@
         <v>2</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F98" s="3"/>
     </row>
@@ -4904,7 +4908,7 @@
         <v>114</v>
       </c>
       <c r="E99" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="112">
@@ -4918,10 +4922,10 @@
         <v>51</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F100" s="3"/>
     </row>
@@ -4936,10 +4940,10 @@
         <v>4</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E101" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F101" s="3"/>
     </row>
@@ -4957,7 +4961,7 @@
         <v>112</v>
       </c>
       <c r="E102" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F102" s="3"/>
     </row>
@@ -4972,16 +4976,16 @@
         <v>6</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E103" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F103" s="3"/>
     </row>
     <row r="104" spans="1:6" ht="31" customHeight="1">
       <c r="A104" s="23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="21"/>
@@ -4991,117 +4995,117 @@
     </row>
     <row r="105" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A105" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E105" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A106" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="E106" s="11" t="s">
         <v>407</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E106" s="11" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="70">
       <c r="A107" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="70">
       <c r="A108" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="70">
       <c r="A109" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E109" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="70">
       <c r="A110" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="70">
       <c r="A111" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="70">
       <c r="A112" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="70">
       <c r="A113" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="70">
       <c r="A114" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="14" customHeight="1">
       <c r="A115" s="24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B115" s="24"/>
       <c r="C115" s="24"/>
@@ -5111,128 +5115,128 @@
     </row>
     <row r="116" spans="1:6" ht="73" customHeight="1">
       <c r="A116" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E116" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="84">
       <c r="A117" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E117" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="84">
       <c r="A118" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D118" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="84">
       <c r="A119" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D119" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="84">
       <c r="A120" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D120" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="84">
       <c r="A121" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D121" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="84">
       <c r="A122" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="84">
       <c r="A123" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D123" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="84">
       <c r="A124" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D124" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="84">
       <c r="A125" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D125" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="84">
       <c r="A126" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D126" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="14" customHeight="1">
       <c r="A127" s="24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B127" s="24"/>
       <c r="C127" s="24"/>
@@ -5242,123 +5246,123 @@
     </row>
     <row r="128" spans="1:6" ht="84">
       <c r="A128" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="84">
       <c r="A129" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="84">
       <c r="A130" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D130" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="84">
       <c r="A131" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D131" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="84">
       <c r="A132" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D132" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="E132" s="11" t="s">
         <v>355</v>
-      </c>
-      <c r="D132" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E132" s="11" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="84">
       <c r="A133" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D133" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="84">
       <c r="A134" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="84">
       <c r="A135" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D135" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="E135" s="11" t="s">
         <v>358</v>
-      </c>
-      <c r="D135" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E135" s="11" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="84">
       <c r="A136" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D136" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="E136" s="11" t="s">
         <v>360</v>
-      </c>
-      <c r="D136" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E136" s="11" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="84">
       <c r="A137" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D137" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="E137" s="11" t="s">
         <v>362</v>
-      </c>
-      <c r="D137" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E137" s="11" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="84">
       <c r="A138" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D138" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sample file update to Municipality violation
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="3200" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="47140" yWindow="1000" windowWidth="28800" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="419">
   <si>
     <t>Description</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>Indicates that the vehicle involved in the incident was carrying hazardous material</t>
-  </si>
-  <si>
-    <t>Local ordinance number that was violated</t>
   </si>
   <si>
     <t>Code of Federal Regulation in violation</t>
@@ -1287,6 +1284,15 @@
   </si>
   <si>
     <t>SL2</t>
+  </si>
+  <si>
+    <t>20-124</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Offense[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Offense']/@s:id]/inc-ext:MunicipalityOrdinanceIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Municipality Ordinance</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1420,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1517,6 +1523,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1527,7 +1539,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="686">
+  <cellStyleXfs count="688">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -2214,8 +2226,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2298,8 +2312,11 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="686">
+  <cellStyles count="688">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2651,6 +2668,7 @@
     <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="687" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2981,6 +2999,7 @@
     <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="686" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -3284,11 +3303,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3305,31 +3324,31 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" ht="18">
       <c r="A1" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="12"/>
@@ -3337,52 +3356,52 @@
     </row>
     <row r="3" spans="1:6" ht="70">
       <c r="A3" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D3" s="2">
         <v>82734800</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A4" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A5" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>413</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>414</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -3391,60 +3410,60 @@
         <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A7" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A8" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="12"/>
@@ -3455,16 +3474,16 @@
         <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3472,16 +3491,16 @@
         <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3489,16 +3508,16 @@
         <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3516,16 +3535,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="84">
@@ -3539,10 +3558,10 @@
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="84">
@@ -3556,10 +3575,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="84">
@@ -3573,10 +3592,10 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" ht="84">
@@ -3593,63 +3612,63 @@
         <v>5495</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="84">
       <c r="A19" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D19" s="2">
         <v>11846050</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="84">
       <c r="A20" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A21" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>296</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -3662,21 +3681,21 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -3686,19 +3705,19 @@
     </row>
     <row r="25" spans="1:6" ht="70">
       <c r="A25" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>228</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3722,10 +3741,10 @@
         <v>12</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="70">
@@ -3739,27 +3758,27 @@
         <v>13</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="70">
       <c r="A29" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="112">
@@ -3773,10 +3792,10 @@
         <v>15</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="112">
@@ -3790,10 +3809,10 @@
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="140">
@@ -3807,10 +3826,10 @@
         <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3827,7 +3846,7 @@
         <v>5401</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="84">
@@ -3844,32 +3863,32 @@
         <v>1209345</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="84">
       <c r="A35" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="70">
       <c r="A36" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>8</v>
@@ -3878,12 +3897,12 @@
         <v>0</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="140">
       <c r="A37" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>55</v>
@@ -3895,7 +3914,7 @@
         <v>12345678</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3903,16 +3922,16 @@
         <v>16</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="3" customFormat="1" ht="112">
@@ -3920,16 +3939,16 @@
         <v>17</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3946,7 +3965,7 @@
         <v>24092</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F40" s="7"/>
     </row>
@@ -3961,27 +3980,27 @@
         <v>59</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A42" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3998,21 +4017,21 @@
         <v>70</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A44" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="3" customFormat="1" ht="70">
@@ -4029,60 +4048,60 @@
         <v>135</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A46" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A47" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A48" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -4095,58 +4114,58 @@
         <v>60</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="3" customFormat="1" ht="112">
       <c r="A51" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="3" customFormat="1" ht="112">
       <c r="A52" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A53" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>24</v>
@@ -4155,97 +4174,97 @@
         <v>2015</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A54" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A55" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="E55" s="11" t="s">
         <v>403</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A56" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A57" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A58" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A59" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>67</v>
@@ -4254,15 +4273,15 @@
         <v>39</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -4272,113 +4291,113 @@
     </row>
     <row r="61" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A61" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A62" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F62" s="7"/>
     </row>
     <row r="63" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A63" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="E63" s="11" t="s">
         <v>265</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D63" s="27" t="s">
-        <v>393</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>266</v>
       </c>
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A64" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D64" s="27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:5" s="3" customFormat="1" ht="126">
       <c r="A65" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A66" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D66" s="27" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A67" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>61</v>
@@ -4387,35 +4406,35 @@
         <v>30</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="3" customFormat="1" ht="42">
       <c r="A68" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="3" customFormat="1" ht="98">
       <c r="A69" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>32</v>
@@ -4424,7 +4443,7 @@
         <v>0.2</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="3" customFormat="1" ht="70">
@@ -4441,21 +4460,21 @@
         <v>30</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A71" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D71" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D71" s="27" t="s">
-        <v>146</v>
-      </c>
       <c r="E71" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="3" customFormat="1" ht="70">
@@ -4472,26 +4491,26 @@
         <v>40</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A73" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D73" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D73" s="27" t="s">
-        <v>146</v>
-      </c>
       <c r="E73" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A74" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>64</v>
@@ -4500,15 +4519,15 @@
         <v>35</v>
       </c>
       <c r="D74" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A75" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>65</v>
@@ -4517,15 +4536,15 @@
         <v>36</v>
       </c>
       <c r="D75" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A76" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>66</v>
@@ -4534,97 +4553,97 @@
         <v>37</v>
       </c>
       <c r="D76" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="3" customFormat="1" ht="70">
       <c r="A77" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>408</v>
+      </c>
+      <c r="E77" s="11" t="s">
         <v>410</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="D77" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="E77" s="11" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="70">
       <c r="A78" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="70">
       <c r="A79" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="70">
       <c r="A80" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="70">
       <c r="A81" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
@@ -4632,34 +4651,34 @@
       <c r="E82" s="13"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" ht="84">
+    <row r="83" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A83" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>68</v>
+        <v>418</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>129</v>
+        <v>278</v>
+      </c>
+      <c r="D83" s="28" t="s">
+        <v>416</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="3" customFormat="1" ht="70">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A84" s="3" t="s">
-        <v>143</v>
+        <v>278</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>69</v>
+        <v>278</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D84" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D84" s="28" t="s">
         <v>128</v>
       </c>
       <c r="E84" s="11" t="s">
@@ -4668,512 +4687,518 @@
     </row>
     <row r="85" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A85" s="3" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>416</v>
+        <v>40</v>
+      </c>
+      <c r="D85" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" ht="98">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A86" s="3" t="s">
-        <v>283</v>
+        <v>104</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>283</v>
+        <v>69</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>395</v>
+      <c r="D86" s="28" t="s">
+        <v>415</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" ht="42">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="3" customFormat="1" ht="98">
       <c r="A87" s="3" t="s">
-        <v>144</v>
+        <v>282</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>167</v>
+        <v>282</v>
       </c>
       <c r="C87" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A88" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D87" s="27" t="s">
-        <v>381</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="F87" s="6"/>
-    </row>
-    <row r="88" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A88" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D88" s="27">
-        <v>2</v>
+      <c r="D88" s="27" t="s">
+        <v>380</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>184</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="F88" s="6"/>
     </row>
     <row r="89" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A89" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D89" s="27" t="s">
-        <v>396</v>
+        <v>41</v>
+      </c>
+      <c r="D89" s="27">
+        <v>2</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="F89" s="8"/>
+        <v>183</v>
+      </c>
     </row>
     <row r="90" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A90" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C90" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D90" s="27" t="s">
+        <v>395</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="F90" s="8"/>
+    </row>
+    <row r="91" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A91" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D90" s="27" t="s">
+      <c r="D91" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F91" s="8"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A93" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A94" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D94" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="E90" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F90" s="8"/>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="5"/>
-    </row>
-    <row r="92" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A92" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E92" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A93" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="E93" s="11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A94" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C94" s="3" t="s">
+      <c r="E94" s="11" t="s">
         <v>213</v>
-      </c>
-      <c r="D94" s="3">
-        <v>12345</v>
-      </c>
-      <c r="E94" s="11" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A95" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D95" s="3">
+        <v>12345</v>
+      </c>
+      <c r="E95" s="11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A96" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E96" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="B95" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D95" s="3" t="s">
+    </row>
+    <row r="97" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A97" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="E97" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" ht="70">
+      <c r="A99" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="E95" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A96" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="E96" s="11" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="13"/>
-      <c r="F97" s="5"/>
-    </row>
-    <row r="98" spans="1:6" ht="70">
-      <c r="A98" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E98" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="F98" s="3"/>
-    </row>
-    <row r="99" spans="1:6" ht="70">
-      <c r="A99" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="112">
-      <c r="A100" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>133</v>
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="1:6" ht="70">
+      <c r="A100" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="F100" s="3"/>
+        <v>176</v>
+      </c>
     </row>
     <row r="101" spans="1:6" ht="112">
       <c r="A101" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:6" ht="112">
+      <c r="A102" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E101" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="F101" s="3"/>
-    </row>
-    <row r="102" spans="1:6" ht="126">
-      <c r="A102" s="3" t="s">
+      <c r="D102" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="1:6" ht="126">
+      <c r="A103" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C103" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E102" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="F102" s="3"/>
-    </row>
-    <row r="103" spans="1:6" ht="112">
-      <c r="A103" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="D103" s="3" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="E103" s="10" t="s">
         <v>202</v>
       </c>
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="1:6" ht="31" customHeight="1">
-      <c r="A104" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="B104" s="21"/>
-      <c r="C104" s="21"/>
-      <c r="D104" s="21"/>
-      <c r="E104" s="22"/>
-      <c r="F104" s="21"/>
-    </row>
-    <row r="105" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A105" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="E105" s="14" t="s">
-        <v>299</v>
-      </c>
+    <row r="104" spans="1:6" ht="112">
+      <c r="A104" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="1:6" ht="31" customHeight="1">
+      <c r="A105" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="B105" s="21"/>
+      <c r="C105" s="21"/>
+      <c r="D105" s="21"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="21"/>
     </row>
     <row r="106" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A106" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A107" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="E107" s="11" t="s">
         <v>406</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="E106" s="11" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="70">
-      <c r="A107" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="E107" s="11" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="70">
       <c r="A108" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="70">
       <c r="A109" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E109" s="11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="70">
       <c r="A110" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="70">
       <c r="A111" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="70">
       <c r="A112" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="70">
       <c r="A113" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="70">
       <c r="A114" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E114" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="70">
+      <c r="A115" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="14" customHeight="1">
+      <c r="A116" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="B116" s="24"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="24"/>
+      <c r="E116" s="25"/>
+      <c r="F116" s="24"/>
+    </row>
+    <row r="117" spans="1:6" ht="73" customHeight="1">
+      <c r="A117" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D117" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="E114" s="11" t="s">
+      <c r="E117" s="11" t="s">
         <v>334</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="14" customHeight="1">
-      <c r="A115" s="24" t="s">
-        <v>325</v>
-      </c>
-      <c r="B115" s="24"/>
-      <c r="C115" s="24"/>
-      <c r="D115" s="24"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="24"/>
-    </row>
-    <row r="116" spans="1:6" ht="73" customHeight="1">
-      <c r="A116" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="E116" s="11" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="84">
-      <c r="A117" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="E117" s="11" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="84">
       <c r="A118" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D118" s="26" t="s">
-        <v>363</v>
+        <v>309</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="84">
       <c r="A119" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D119" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="84">
       <c r="A120" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D120" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="84">
       <c r="A121" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D121" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E121" s="11" t="s">
         <v>339</v>
@@ -5181,188 +5206,199 @@
     </row>
     <row r="122" spans="1:6" ht="84">
       <c r="A122" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>375</v>
+        <v>313</v>
+      </c>
+      <c r="D122" s="26" t="s">
+        <v>362</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="84">
       <c r="A123" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="D123" s="26" t="s">
-        <v>363</v>
+        <v>314</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>374</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="84">
       <c r="A124" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D124" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="84">
       <c r="A125" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D125" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="84">
       <c r="A126" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D126" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="14" customHeight="1">
-      <c r="A127" s="24" t="s">
-        <v>326</v>
-      </c>
-      <c r="B127" s="24"/>
-      <c r="C127" s="24"/>
-      <c r="D127" s="24"/>
-      <c r="E127" s="25"/>
-      <c r="F127" s="24"/>
-    </row>
-    <row r="128" spans="1:6" ht="84">
-      <c r="A128" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="E128" s="11" t="s">
-        <v>346</v>
-      </c>
+        <v>343</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="84">
+      <c r="A127" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D127" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="E127" s="11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="14" customHeight="1">
+      <c r="A128" s="24" t="s">
+        <v>325</v>
+      </c>
+      <c r="B128" s="24"/>
+      <c r="C128" s="24"/>
+      <c r="D128" s="24"/>
+      <c r="E128" s="25"/>
+      <c r="F128" s="24"/>
     </row>
     <row r="129" spans="1:5" ht="84">
       <c r="A129" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="84">
       <c r="A130" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="D130" s="26" t="s">
-        <v>363</v>
+        <v>320</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="84">
       <c r="A131" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D131" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="E131" s="11" t="s">
         <v>351</v>
-      </c>
-      <c r="D131" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="E131" s="11" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="84">
       <c r="A132" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D132" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="84">
       <c r="A133" s="2" t="s">
-        <v>322</v>
+        <v>353</v>
       </c>
       <c r="D133" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="84">
       <c r="A134" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>377</v>
+        <v>321</v>
+      </c>
+      <c r="D134" s="26" t="s">
+        <v>362</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="84">
       <c r="A135" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="D135" s="26" t="s">
-        <v>363</v>
+        <v>322</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="84">
       <c r="A136" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D136" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E136" s="11" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="84">
       <c r="A137" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D137" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E137" s="11" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="84">
       <c r="A138" s="2" t="s">
-        <v>324</v>
+        <v>360</v>
       </c>
       <c r="D138" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>350</v>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="84">
+      <c r="A139" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D139" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="E139" s="11" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Arrest elements to Arrest Reporting NIEM subset.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="47140" yWindow="1000" windowWidth="28800" windowHeight="16500"/>
+    <workbookView xWindow="6040" yWindow="1320" windowWidth="22280" windowHeight="15920"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="500">
   <si>
     <t>Description</t>
   </si>
@@ -1271,9 +1271,6 @@
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityDocument/nc:Document/@s:id]/inc-ext:SeatBeltViolationCount</t>
   </si>
   <si>
-    <t>Citation Violation Date</t>
-  </si>
-  <si>
     <t>The date of the violation</t>
   </si>
   <si>
@@ -1293,6 +1290,252 @@
   </si>
   <si>
     <t>Municipality Ordinance</t>
+  </si>
+  <si>
+    <t>Spillman</t>
+  </si>
+  <si>
+    <t>CTMAIN TABLE/ CTMDESC.TEXT</t>
+  </si>
+  <si>
+    <t>CTMAIN TABLE/CTMDESC.TEXT</t>
+  </si>
+  <si>
+    <t>NMMAIN.DLNUMB</t>
+  </si>
+  <si>
+    <t>NMLOCAL.LOCALID</t>
+  </si>
+  <si>
+    <t>NMMAIN.LAST</t>
+  </si>
+  <si>
+    <t>NMMAIN.FIRST</t>
+  </si>
+  <si>
+    <t>NMMAIN.MIDDLE</t>
+  </si>
+  <si>
+    <t>CTMAIN TABLE/ CTMDESC.TEXT (may need to change the form in TRACS so officer can signify that the mailing adddress is also the physical address. If it's different , we may need to add a physical address field in TraCS)</t>
+  </si>
+  <si>
+    <t>NMMAIN.PHONE</t>
+  </si>
+  <si>
+    <t>NMMAIN.WRKPHN</t>
+  </si>
+  <si>
+    <t>NMMAIN.BIRTHD</t>
+  </si>
+  <si>
+    <t>NMMAIN.SEX</t>
+  </si>
+  <si>
+    <t>NMEXTRA.BCITY</t>
+  </si>
+  <si>
+    <t>NMMAIN.HEIGHT</t>
+  </si>
+  <si>
+    <t>NMMAIN.WEIGHT</t>
+  </si>
+  <si>
+    <t>NMMAIN.HAIR</t>
+  </si>
+  <si>
+    <t>NNMAIN.EYES</t>
+  </si>
+  <si>
+    <t>VHMAIN.LPST</t>
+  </si>
+  <si>
+    <t>VHMAIN.YEAR</t>
+  </si>
+  <si>
+    <t>VHMAIN.MAKE</t>
+  </si>
+  <si>
+    <t>VHMAIN.MODEL</t>
+  </si>
+  <si>
+    <t>VHMAIN.COLOR1</t>
+  </si>
+  <si>
+    <t>CTMAIN.VILDATE</t>
+  </si>
+  <si>
+    <t>Citation Violation Date/Time</t>
+  </si>
+  <si>
+    <t>CTMAIN.AGENCY</t>
+  </si>
+  <si>
+    <t>CTMAIN.STREET</t>
+  </si>
+  <si>
+    <t>CTMAIN.SPACT</t>
+  </si>
+  <si>
+    <t>CTMAIN.SPPOST</t>
+  </si>
+  <si>
+    <t>CTMAIN.ISSUOFF</t>
+  </si>
+  <si>
+    <t>CTMAIN.BONDAMT</t>
+  </si>
+  <si>
+    <t>CTMAIN.DTISSUE</t>
+  </si>
+  <si>
+    <t>MasterCitationTable/CitationNumber</t>
+  </si>
+  <si>
+    <t>MasterCitationTable/DateOfCitation</t>
+  </si>
+  <si>
+    <t>MasterCitationTable/BondAmount</t>
+  </si>
+  <si>
+    <t>CommentsForCitationRecords/MiscellaneousComments</t>
+  </si>
+  <si>
+    <t>MasterCitationTable/AgencyCode</t>
+  </si>
+  <si>
+    <t>MasterCitationTable/StreetAddress</t>
+  </si>
+  <si>
+    <t>MainNamesTable/LastName</t>
+  </si>
+  <si>
+    <t>MainNamesTable/FirstName</t>
+  </si>
+  <si>
+    <t>MainNamesTable/MiddleName</t>
+  </si>
+  <si>
+    <t>MainNamesTable/StreetAddress</t>
+  </si>
+  <si>
+    <t>MainNamesTable/CityOfResidence</t>
+  </si>
+  <si>
+    <t>MainNamesTable/StateAbbreviation</t>
+  </si>
+  <si>
+    <t>MainNamesTable/ZipCode</t>
+  </si>
+  <si>
+    <t>MainNamesTable/DriverLicenseNumber</t>
+  </si>
+  <si>
+    <t>MainNamesTable/DriverLicenseState</t>
+  </si>
+  <si>
+    <t>NMMAIN.DLSTATE</t>
+  </si>
+  <si>
+    <t>NameLocalIDDetail/LocalIDNumber</t>
+  </si>
+  <si>
+    <t>MainNamesTable/HomePhoneNumber</t>
+  </si>
+  <si>
+    <t>MainNamesTable/WorkTelephoneNumber</t>
+  </si>
+  <si>
+    <t>MainNamesTable/BirthDate</t>
+  </si>
+  <si>
+    <t>MainNamesTable/Sex</t>
+  </si>
+  <si>
+    <t>AdditionalNameInformation/CityOfBirth</t>
+  </si>
+  <si>
+    <t>MainNamesTable/Height</t>
+  </si>
+  <si>
+    <t>MainNamesTable/Weight</t>
+  </si>
+  <si>
+    <t>MainNamesTable/Hair</t>
+  </si>
+  <si>
+    <t>MainNamesTable/Eye</t>
+  </si>
+  <si>
+    <t>MainVehicleScreen/LicensePlateNumber</t>
+  </si>
+  <si>
+    <t>VHMAIN.LPNUM</t>
+  </si>
+  <si>
+    <t>MainVehicleScreen/LicenseStateAbbreviation</t>
+  </si>
+  <si>
+    <t>MainVehicleScreen/YearOfCar</t>
+  </si>
+  <si>
+    <t>MainVehicleScreen/MakeOfCar</t>
+  </si>
+  <si>
+    <t>MainVehicleScreen/ModelOfCar</t>
+  </si>
+  <si>
+    <t>MainVehicleScreen/ColorPrimary</t>
+  </si>
+  <si>
+    <t>MasterCitationTable/Posted</t>
+  </si>
+  <si>
+    <t>MasterCitationTable/Actual</t>
+  </si>
+  <si>
+    <t>MasterCitationTable/IssuingOfficer</t>
+  </si>
+  <si>
+    <t>MasterCitationTable/ViolationDate</t>
+  </si>
+  <si>
+    <t>LawIncidentTable/IncidentNumber</t>
+  </si>
+  <si>
+    <t>LWMAIN.NUMBER</t>
+  </si>
+  <si>
+    <t>LawIncidentTable/TimeDateOccurredAfter</t>
+  </si>
+  <si>
+    <t>LWMAIN.OCURDT1</t>
+  </si>
+  <si>
+    <t>LawIncidentTable/TimeDateOccurredBefore</t>
+  </si>
+  <si>
+    <t>LWMAIN.OCURDT2</t>
+  </si>
+  <si>
+    <t>LawIncidentNarrative/Narrative</t>
+  </si>
+  <si>
+    <t>LWNARR.NARRATV</t>
+  </si>
+  <si>
+    <t>LawIncidentTable/City</t>
+  </si>
+  <si>
+    <t>LWMAIN.CITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTMAIN.NUMBER </t>
+  </si>
+  <si>
+    <t>varname</t>
+  </si>
+  <si>
+    <t>Tag</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1545,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1419,8 +1662,50 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1529,6 +1814,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1539,7 +1830,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="688">
+  <cellStyleXfs count="834">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -2228,8 +2519,154 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2315,8 +2752,44 @@
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="688">
+  <cellStyles count="834">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2669,6 +3142,79 @@
     <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="687" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="689" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="691" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="693" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="695" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="697" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="699" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="701" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="703" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="709" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="711" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="719" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="721" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="739" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="741" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="743" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="751" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="773" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="775" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="777" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="779" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="787" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="789" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="793" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="795" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="797" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="799" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="801" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="803" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="805" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="807" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="809" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="811" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="813" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="815" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="817" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="819" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="821" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="823" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="825" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="827" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="829" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="831" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="833" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -3000,6 +3546,79 @@
     <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="686" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="688" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="690" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="692" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="694" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="696" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="698" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="700" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="702" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="704" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="706" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="708" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="710" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="712" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="714" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="716" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="718" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="720" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="722" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="728" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="730" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="738" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="740" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="742" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="744" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="746" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="748" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="750" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="752" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="754" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="766" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="768" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="770" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="772" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="774" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="776" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="778" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="786" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="788" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="792" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="794" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="796" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="798" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="800" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="802" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="804" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="806" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="808" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="810" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="812" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="814" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="816" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="818" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="820" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="822" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="824" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="826" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="828" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="830" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="832" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -3303,2101 +3922,2623 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="105.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="57.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.1640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="27.1640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="39.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="105.83203125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="57.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.1640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="9" customFormat="1" ht="18">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="18">
+      <c r="A1" s="29" t="s">
+        <v>418</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="12"/>
       <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="70">
-      <c r="A3" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>156</v>
+      <c r="G2" s="12"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="70">
+      <c r="A3" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>450</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="2">
         <v>82734800</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A4" s="32" t="s">
+        <v>449</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>451</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A5" s="3" t="s">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A5" s="32" t="s">
+        <v>441</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>486</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>157</v>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A6" s="32" t="s">
+        <v>448</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>452</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="27" t="s">
         <v>379</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A7" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>174</v>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A7" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>362</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A8" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>175</v>
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A8" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="12"/>
       <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="112" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>218</v>
+      <c r="G9" s="12"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" ht="112" customHeight="1">
+      <c r="A10" s="33" t="s">
+        <v>443</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>454</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>217</v>
+    <row r="11" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A11" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>219</v>
+    <row r="12" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A12" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>455</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="70">
-      <c r="A14" s="17" t="s">
+      <c r="G13" s="13"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="70">
+      <c r="A14" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="C14" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="84">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:8" ht="84">
+      <c r="C15" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="84">
-      <c r="A16" s="20" t="s">
+    <row r="16" spans="1:8" ht="84">
+      <c r="C16" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="84">
-      <c r="A17" s="20" t="s">
+    <row r="17" spans="1:8" ht="84">
+      <c r="C17" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:8" s="3" customFormat="1" ht="84">
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="3">
+      <c r="F18" s="3">
         <v>5495</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="84">
-      <c r="A19" s="17" t="s">
+    <row r="19" spans="1:8" ht="84">
+      <c r="C19" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="D19" s="2">
+      <c r="F19" s="2">
         <v>11846050</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="G19" s="10" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="84">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:8" ht="84">
+      <c r="C20" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:8" s="3" customFormat="1" ht="84">
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="15" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15" t="s">
         <v>384</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" ht="70">
-      <c r="A23" s="20" t="s">
+      <c r="G22" s="13"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="70">
+      <c r="A23" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B23" s="33"/>
+      <c r="C23" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="G23" s="10" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="15" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="13"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" ht="70">
-      <c r="A25" s="2" t="s">
+      <c r="G24" s="13"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" ht="70">
+      <c r="A25" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="G25" s="10" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="15" t="s">
+    <row r="26" spans="1:8">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" ht="70">
-      <c r="A27" s="2" t="s">
+      <c r="G26" s="13"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" ht="70">
+      <c r="A27" s="33" t="s">
+        <v>423</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>456</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="G27" s="10" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="70">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:8" ht="70">
+      <c r="A28" s="33" t="s">
+        <v>424</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>457</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="G28" s="10" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="70">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:8" ht="70">
+      <c r="A29" s="33" t="s">
+        <v>425</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>458</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="G29" s="14" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="112">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:8" ht="112">
+      <c r="A30" s="39" t="s">
+        <v>426</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>459</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="G30" s="10" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="112">
-      <c r="A31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>4</v>
+    <row r="31" spans="1:8" ht="112">
+      <c r="A31" s="39" t="s">
+        <v>419</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>460</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="G31" s="10" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="140">
-      <c r="A32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>5</v>
+    <row r="32" spans="1:8" ht="140">
+      <c r="A32" s="39" t="s">
+        <v>419</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>461</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="G32" s="10" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>6</v>
+    <row r="33" spans="1:8" s="3" customFormat="1" ht="112">
+      <c r="A33" s="39" t="s">
+        <v>419</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>462</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="3">
         <v>5401</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="G33" s="11" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="84">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:8" ht="84">
+      <c r="A34" s="32" t="s">
+        <v>421</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>463</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="2">
+      <c r="F34" s="2">
         <v>1209345</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="G34" s="14" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="84">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:8" ht="84">
+      <c r="A35" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>464</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="G35" s="14" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="70">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:8" ht="70">
+      <c r="A36" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="2" t="b">
+      <c r="F36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="G36" s="10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="140">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:8" ht="140">
+      <c r="A37" s="33" t="s">
+        <v>422</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="2">
+      <c r="F37" s="2">
         <v>12345678</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="G37" s="14" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>160</v>
+    <row r="38" spans="1:8" s="3" customFormat="1" ht="112">
+      <c r="A38" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>467</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="G38" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>161</v>
+    <row r="39" spans="1:8" s="3" customFormat="1" ht="112">
+      <c r="A39" s="33" t="s">
+        <v>428</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>468</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>18</v>
+    <row r="40" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A40" s="33" t="s">
+        <v>429</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>469</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="7">
         <v>24092</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="G40" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>59</v>
+      <c r="H40" s="7"/>
+    </row>
+    <row r="41" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A41" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>470</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="G41" s="14" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:8" s="3" customFormat="1" ht="84">
+      <c r="A42" s="33" t="s">
+        <v>431</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>471</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="G42" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>20</v>
+    <row r="43" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A43" s="33" t="s">
+        <v>432</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>472</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="3">
         <v>70</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="G43" s="14" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A44" s="31"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="G44" s="14" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A45" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>21</v>
+    <row r="45" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A45" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>473</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="3">
         <v>135</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="G45" s="14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A46" s="31"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="G46" s="14" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A47" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="G47" s="14" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A48" s="33" t="s">
+        <v>435</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="G48" s="14" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="15" t="s">
+    <row r="49" spans="1:8">
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="13"/>
+      <c r="E49" s="5"/>
       <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>122</v>
-      </c>
+      <c r="G49" s="13"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" s="3" customFormat="1" ht="98">
+      <c r="A50" s="31"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="G50" s="11" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:8" s="3" customFormat="1" ht="112">
+      <c r="A51" s="33" t="s">
+        <v>477</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>476</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="G51" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="3" customFormat="1" ht="112">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:8" s="3" customFormat="1" ht="112">
+      <c r="A52" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="B52" s="33" t="s">
+        <v>478</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="G52" s="11" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:8" s="3" customFormat="1" ht="98">
+      <c r="A53" s="33" t="s">
+        <v>437</v>
+      </c>
+      <c r="B53" s="33" t="s">
+        <v>479</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="3">
+      <c r="F53" s="3">
         <v>2015</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="G53" s="11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:8" s="3" customFormat="1" ht="98">
+      <c r="A54" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="B54" s="33" t="s">
+        <v>480</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="G54" s="11" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:8" s="3" customFormat="1" ht="98">
+      <c r="A55" s="33" t="s">
+        <v>439</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="F55" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="G55" s="11" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:8" s="3" customFormat="1" ht="98">
+      <c r="A56" s="33" t="s">
+        <v>440</v>
+      </c>
+      <c r="B56" s="33" t="s">
+        <v>482</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="G56" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:8" s="3" customFormat="1" ht="98">
+      <c r="A57" s="31"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="G57" s="11" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="58" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A58" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B58" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D58" s="27" t="s">
+      <c r="F58" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="G58" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A59" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B59" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D59" s="27" t="s">
+      <c r="F59" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="G59" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="15" t="s">
+    <row r="60" spans="1:8">
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="13"/>
+      <c r="E60" s="5"/>
       <c r="F60" s="5"/>
-    </row>
-    <row r="61" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A61" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>154</v>
+      <c r="G60" s="13"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" s="3" customFormat="1" ht="42">
+      <c r="A61" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>487</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E61" s="11" t="s">
+      <c r="G61" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A62" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>263</v>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" s="3" customFormat="1" ht="42">
+      <c r="A62" s="30" t="s">
+        <v>490</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>489</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D62" s="27" t="s">
+      <c r="D62" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F62" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="E62" s="11" t="s">
+      <c r="G62" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A63" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>264</v>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" s="3" customFormat="1" ht="42">
+      <c r="A63" s="30" t="s">
+        <v>492</v>
+      </c>
+      <c r="B63" s="30" t="s">
+        <v>491</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D63" s="27" t="s">
+      <c r="D63" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="F63" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="G63" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="F63" s="7"/>
-    </row>
-    <row r="64" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A64" s="3" t="s">
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="1:8" s="35" customFormat="1" ht="70">
+      <c r="A64" s="40" t="s">
+        <v>494</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="C64" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="D64" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="E64" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D64" s="27" t="s">
+      <c r="F64" s="36" t="s">
         <v>393</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="G64" s="37" t="s">
         <v>285</v>
       </c>
-      <c r="F64" s="7"/>
-    </row>
-    <row r="65" spans="1:5" s="3" customFormat="1" ht="126">
-      <c r="A65" s="3" t="s">
+      <c r="H64" s="38"/>
+    </row>
+    <row r="65" spans="1:7" s="3" customFormat="1" ht="126">
+      <c r="A65" s="33" t="s">
+        <v>496</v>
+      </c>
+      <c r="B65" s="30" t="s">
+        <v>495</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D65" s="27" t="s">
+      <c r="F65" s="27" t="s">
         <v>381</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="G65" s="11" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A66" s="3" t="s">
+    <row r="66" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A66" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B66" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="27" t="s">
+      <c r="F66" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="G66" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A67" s="3" t="s">
+    <row r="67" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A67" s="32" t="s">
+        <v>444</v>
+      </c>
+      <c r="B67" s="32" t="s">
+        <v>455</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="E67" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D67" s="27" t="s">
+      <c r="F67" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="E67" s="11" t="s">
+      <c r="G67" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="3" customFormat="1" ht="42">
-      <c r="A68" s="3" t="s">
+    <row r="68" spans="1:7" s="3" customFormat="1" ht="42">
+      <c r="A68" s="33" t="s">
+        <v>494</v>
+      </c>
+      <c r="B68" s="30" t="s">
+        <v>493</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D68" s="27" t="s">
+      <c r="F68" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="E68" s="11" t="s">
+      <c r="G68" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="3" customFormat="1" ht="98">
-      <c r="A69" s="3" t="s">
+    <row r="69" spans="1:7" s="3" customFormat="1" ht="98">
+      <c r="A69" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B69" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D69" s="27">
+      <c r="F69" s="27">
         <v>0.2</v>
       </c>
-      <c r="E69" s="11" t="s">
+      <c r="G69" s="11" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A70" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>62</v>
+    <row r="70" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A70" s="32" t="s">
+        <v>445</v>
+      </c>
+      <c r="B70" s="32" t="s">
+        <v>484</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="27">
+      <c r="D70" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F70" s="27">
         <v>30</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="G70" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A71" s="3" t="s">
+    <row r="71" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A71" s="31"/>
+      <c r="B71" s="31"/>
+      <c r="C71" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D71" s="27" t="s">
+      <c r="F71" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="G71" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A72" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>63</v>
+    <row r="72" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A72" s="32" t="s">
+        <v>446</v>
+      </c>
+      <c r="B72" s="32" t="s">
+        <v>483</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D72" s="27">
+      <c r="D72" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F72" s="27">
         <v>40</v>
       </c>
-      <c r="E72" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A73" s="3" t="s">
+    <row r="73" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A73" s="31"/>
+      <c r="B73" s="31"/>
+      <c r="C73" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D73" s="27" t="s">
+      <c r="F73" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="E73" s="11" t="s">
+      <c r="G73" s="11" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A74" s="3" t="s">
+    <row r="74" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A74" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B74" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="D74" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="E74" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D74" s="27" t="s">
+      <c r="F74" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E74" s="11" t="s">
+      <c r="G74" s="11" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A75" s="3" t="s">
+    <row r="75" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A75" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B75" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D75" s="27" t="s">
+      <c r="F75" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E75" s="11" t="s">
+      <c r="G75" s="11" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A76" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B76" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="D76" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="E76" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D76" s="27" t="s">
+      <c r="F76" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E76" s="11" t="s">
+      <c r="G76" s="11" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="3" customFormat="1" ht="70">
-      <c r="A77" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>407</v>
+    <row r="77" spans="1:7" s="3" customFormat="1" ht="70">
+      <c r="A77" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B77" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="D77" s="27" t="s">
+      <c r="D77" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="F77" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="E77" s="11" t="s">
+      <c r="G77" s="11" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="70">
-      <c r="A78" s="2" t="s">
+    <row r="78" spans="1:7" ht="70">
+      <c r="A78" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B78" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D78" s="26" t="s">
+      <c r="F78" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="G78" s="11" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="70">
-      <c r="A79" s="2" t="s">
+    <row r="79" spans="1:7" ht="70">
+      <c r="A79" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B79" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D79" s="26" t="s">
+      <c r="F79" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E79" s="11" t="s">
+      <c r="G79" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="70">
-      <c r="A80" s="2" t="s">
+    <row r="80" spans="1:7" ht="70">
+      <c r="A80" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B80" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="E80" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D80" s="26" t="s">
+      <c r="F80" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E80" s="11" t="s">
+      <c r="G80" s="11" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="70">
-      <c r="A81" s="2" t="s">
+    <row r="81" spans="1:8" ht="70">
+      <c r="A81" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B81" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D81" s="26" t="s">
+      <c r="F81" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="E81" s="11" t="s">
+      <c r="G81" s="11" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="15" t="s">
+    <row r="82" spans="1:8">
+      <c r="A82" s="15"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
       <c r="D82" s="5"/>
-      <c r="E82" s="13"/>
+      <c r="E82" s="5"/>
       <c r="F82" s="5"/>
-    </row>
-    <row r="83" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A83" s="3" t="s">
+      <c r="G82" s="13"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A83" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B83" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B83" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="C83" s="3" t="s">
+      <c r="D83" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="E83" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="D83" s="28" t="s">
+      <c r="F83" s="28" t="s">
+        <v>415</v>
+      </c>
+      <c r="G83" s="11" t="s">
         <v>416</v>
       </c>
-      <c r="E83" s="11" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A84" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>278</v>
+    </row>
+    <row r="84" spans="1:8" s="3" customFormat="1" ht="84">
+      <c r="A84" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B84" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="D84" s="28" t="s">
+      <c r="D84" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F84" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="E84" s="11" t="s">
+      <c r="G84" s="11" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A85" s="3" t="s">
+    <row r="85" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A85" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B85" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="D85" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="E85" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D85" s="28" t="s">
+      <c r="F85" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="E85" s="11" t="s">
+      <c r="G85" s="11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A86" s="3" t="s">
+    <row r="86" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A86" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B86" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="D86" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="E86" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D86" s="28" t="s">
-        <v>415</v>
-      </c>
-      <c r="E86" s="11" t="s">
+      <c r="F86" s="28" t="s">
+        <v>414</v>
+      </c>
+      <c r="G86" s="11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A87" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>282</v>
+    <row r="87" spans="1:8" s="3" customFormat="1" ht="98">
+      <c r="A87" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B87" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>282</v>
       </c>
       <c r="D87" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="F87" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="G87" s="11" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="88" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A88" s="3" t="s">
+    <row r="88" spans="1:8" s="3" customFormat="1" ht="42">
+      <c r="A88" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="B88" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="D88" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D88" s="27" t="s">
+      <c r="F88" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E88" s="11" t="s">
+      <c r="G88" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="F88" s="6"/>
-    </row>
-    <row r="89" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A89" s="3" t="s">
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A89" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B89" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="D89" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="E89" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D89" s="27">
+      <c r="F89" s="27">
         <v>2</v>
       </c>
-      <c r="E89" s="11" t="s">
+      <c r="G89" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A90" s="3" t="s">
+    <row r="90" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A90" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B90" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="D90" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="E90" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D90" s="27" t="s">
+      <c r="F90" s="27" t="s">
         <v>395</v>
       </c>
-      <c r="E90" s="11" t="s">
+      <c r="G90" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="F90" s="8"/>
-    </row>
-    <row r="91" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A91" s="3" t="s">
+      <c r="H90" s="8"/>
+    </row>
+    <row r="91" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A91" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B91" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="D91" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="E91" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D91" s="27" t="s">
+      <c r="F91" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="E91" s="11" t="s">
+      <c r="G91" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="F91" s="8"/>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" s="15" t="s">
+      <c r="H91" s="8"/>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="15"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
       <c r="D92" s="5"/>
-      <c r="E92" s="13"/>
+      <c r="E92" s="5"/>
       <c r="F92" s="5"/>
-    </row>
-    <row r="93" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A93" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>46</v>
+      <c r="G92" s="13"/>
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A93" s="32" t="s">
+        <v>447</v>
+      </c>
+      <c r="B93" s="32" t="s">
+        <v>485</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D93" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E93" s="11" t="s">
+      <c r="G93" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A94" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>211</v>
+    <row r="94" spans="1:8" s="3" customFormat="1" ht="42">
+      <c r="A94" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B94" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>210</v>
       </c>
       <c r="D94" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="E94" s="11" t="s">
+      <c r="G94" s="11" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A95" s="3" t="s">
+    <row r="95" spans="1:8" s="3" customFormat="1" ht="84">
+      <c r="A95" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="B95" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="D95" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="E95" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D95" s="3">
+      <c r="F95" s="3">
         <v>12345</v>
       </c>
-      <c r="E95" s="11" t="s">
+      <c r="G95" s="11" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A96" s="3" t="s">
+    <row r="96" spans="1:8" s="3" customFormat="1" ht="84">
+      <c r="A96" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B96" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="F96" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E96" s="11" t="s">
+      <c r="G96" s="11" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A97" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>48</v>
+    <row r="97" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A97" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B97" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D97" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="E97" s="11" t="s">
+      <c r="G97" s="11" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="15" t="s">
+    <row r="98" spans="1:8">
+      <c r="A98" s="15"/>
+      <c r="B98" s="15"/>
+      <c r="C98" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
       <c r="D98" s="5"/>
-      <c r="E98" s="13"/>
+      <c r="E98" s="5"/>
       <c r="F98" s="5"/>
-    </row>
-    <row r="99" spans="1:6" ht="70">
-      <c r="A99" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>2</v>
+      <c r="G98" s="13"/>
+      <c r="H98" s="5"/>
+    </row>
+    <row r="99" spans="1:8" ht="70">
+      <c r="A99" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B99" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D99" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E99" s="10" t="s">
+      <c r="G99" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="F99" s="3"/>
-    </row>
-    <row r="100" spans="1:6" ht="70">
-      <c r="A100" s="2" t="s">
+      <c r="H99" s="3"/>
+    </row>
+    <row r="100" spans="1:8" ht="70">
+      <c r="A100" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B100" s="33" t="s">
+        <v>453</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="E100" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="F100" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E100" s="10" t="s">
+      <c r="G100" s="10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="112">
-      <c r="A101" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>51</v>
+    <row r="101" spans="1:8" ht="112">
+      <c r="A101" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B101" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D101" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E101" s="10" t="s">
+      <c r="G101" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="F101" s="3"/>
-    </row>
-    <row r="102" spans="1:6" ht="112">
-      <c r="A102" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>4</v>
+      <c r="H101" s="3"/>
+    </row>
+    <row r="102" spans="1:8" ht="112">
+      <c r="A102" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B102" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D102" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E102" s="10" t="s">
+      <c r="G102" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="F102" s="3"/>
-    </row>
-    <row r="103" spans="1:6" ht="126">
-      <c r="A103" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>5</v>
+      <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="1:8" ht="126">
+      <c r="A103" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B103" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D103" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F103" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E103" s="10" t="s">
+      <c r="G103" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="F103" s="3"/>
-    </row>
-    <row r="104" spans="1:6" ht="112">
-      <c r="A104" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>6</v>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="1:8" ht="112">
+      <c r="A104" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="B104" s="33" t="s">
+        <v>453</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D104" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F104" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E104" s="10" t="s">
+      <c r="G104" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="F104" s="3"/>
-    </row>
-    <row r="105" spans="1:6" ht="31" customHeight="1">
-      <c r="A105" s="23" t="s">
+      <c r="H104" s="3"/>
+    </row>
+    <row r="105" spans="1:8" ht="31" customHeight="1">
+      <c r="C105" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="B105" s="21"/>
-      <c r="C105" s="21"/>
       <c r="D105" s="21"/>
-      <c r="E105" s="22"/>
+      <c r="E105" s="21"/>
       <c r="F105" s="21"/>
-    </row>
-    <row r="106" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A106" s="3" t="s">
+      <c r="G105" s="22"/>
+      <c r="H105" s="21"/>
+    </row>
+    <row r="106" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A106" s="30"/>
+      <c r="B106" s="30"/>
+      <c r="C106" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="F106" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="E106" s="14" t="s">
+      <c r="G106" s="14" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="107" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A107" s="3" t="s">
+    <row r="107" spans="1:8" s="3" customFormat="1" ht="70">
+      <c r="A107" s="30"/>
+      <c r="B107" s="30"/>
+      <c r="C107" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="F107" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E107" s="11" t="s">
+      <c r="G107" s="11" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="70">
-      <c r="A108" s="2" t="s">
+    <row r="108" spans="1:8" ht="70">
+      <c r="C108" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="F108" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="E108" s="11" t="s">
+      <c r="G108" s="11" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="70">
-      <c r="A109" s="2" t="s">
+    <row r="109" spans="1:8" ht="70">
+      <c r="C109" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="F109" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="E109" s="11" t="s">
+      <c r="G109" s="11" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="70">
-      <c r="A110" s="2" t="s">
+    <row r="110" spans="1:8" ht="70">
+      <c r="C110" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D110" s="2" t="s">
+      <c r="F110" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E110" s="11" t="s">
+      <c r="G110" s="11" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="70">
-      <c r="A111" s="2" t="s">
+    <row r="111" spans="1:8" ht="70">
+      <c r="C111" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="F111" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E111" s="11" t="s">
+      <c r="G111" s="11" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="70">
-      <c r="A112" s="2" t="s">
+    <row r="112" spans="1:8" ht="70">
+      <c r="C112" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="F112" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="G112" s="11" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="70">
-      <c r="A113" s="2" t="s">
+    <row r="113" spans="3:8" ht="70">
+      <c r="C113" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="F113" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="E113" s="11" t="s">
+      <c r="G113" s="11" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="70">
-      <c r="A114" s="2" t="s">
+    <row r="114" spans="3:8" ht="70">
+      <c r="C114" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="F114" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="E114" s="11" t="s">
+      <c r="G114" s="11" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="70">
-      <c r="A115" s="2" t="s">
+    <row r="115" spans="3:8" ht="70">
+      <c r="C115" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="F115" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="E115" s="11" t="s">
+      <c r="G115" s="11" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="14" customHeight="1">
-      <c r="A116" s="24" t="s">
+    <row r="116" spans="3:8" ht="14" customHeight="1">
+      <c r="C116" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="B116" s="24"/>
-      <c r="C116" s="24"/>
       <c r="D116" s="24"/>
-      <c r="E116" s="25"/>
+      <c r="E116" s="24"/>
       <c r="F116" s="24"/>
-    </row>
-    <row r="117" spans="1:6" ht="73" customHeight="1">
-      <c r="A117" s="2" t="s">
+      <c r="G116" s="25"/>
+      <c r="H116" s="24"/>
+    </row>
+    <row r="117" spans="3:8" ht="73" customHeight="1">
+      <c r="C117" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="F117" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="E117" s="11" t="s">
+      <c r="G117" s="11" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="84">
-      <c r="A118" s="2" t="s">
+    <row r="118" spans="3:8" ht="84">
+      <c r="C118" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="F118" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E118" s="11" t="s">
+      <c r="G118" s="11" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="84">
-      <c r="A119" s="2" t="s">
+    <row r="119" spans="3:8" ht="84">
+      <c r="C119" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D119" s="26" t="s">
+      <c r="F119" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E119" s="11" t="s">
+      <c r="G119" s="11" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="84">
-      <c r="A120" s="2" t="s">
+    <row r="120" spans="3:8" ht="84">
+      <c r="C120" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D120" s="26" t="s">
+      <c r="F120" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E120" s="11" t="s">
+      <c r="G120" s="11" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="84">
-      <c r="A121" s="2" t="s">
+    <row r="121" spans="3:8" ht="84">
+      <c r="C121" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D121" s="26" t="s">
+      <c r="F121" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E121" s="11" t="s">
+      <c r="G121" s="11" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="84">
-      <c r="A122" s="2" t="s">
+    <row r="122" spans="3:8" ht="84">
+      <c r="C122" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D122" s="26" t="s">
+      <c r="F122" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E122" s="11" t="s">
+      <c r="G122" s="11" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="84">
-      <c r="A123" s="2" t="s">
+    <row r="123" spans="3:8" ht="84">
+      <c r="C123" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="F123" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E123" s="11" t="s">
+      <c r="G123" s="11" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="84">
-      <c r="A124" s="2" t="s">
+    <row r="124" spans="3:8" ht="84">
+      <c r="C124" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D124" s="26" t="s">
+      <c r="F124" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E124" s="11" t="s">
+      <c r="G124" s="11" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="84">
-      <c r="A125" s="2" t="s">
+    <row r="125" spans="3:8" ht="84">
+      <c r="C125" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D125" s="26" t="s">
+      <c r="F125" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E125" s="11" t="s">
+      <c r="G125" s="11" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="84">
-      <c r="A126" s="2" t="s">
+    <row r="126" spans="3:8" ht="84">
+      <c r="C126" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D126" s="26" t="s">
+      <c r="F126" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E126" s="11" t="s">
+      <c r="G126" s="11" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="84">
-      <c r="A127" s="2" t="s">
+    <row r="127" spans="3:8" ht="84">
+      <c r="C127" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D127" s="26" t="s">
+      <c r="F127" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E127" s="11" t="s">
+      <c r="G127" s="11" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="14" customHeight="1">
-      <c r="A128" s="24" t="s">
+    <row r="128" spans="3:8" ht="14" customHeight="1">
+      <c r="C128" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="B128" s="24"/>
-      <c r="C128" s="24"/>
       <c r="D128" s="24"/>
-      <c r="E128" s="25"/>
+      <c r="E128" s="24"/>
       <c r="F128" s="24"/>
-    </row>
-    <row r="129" spans="1:5" ht="84">
-      <c r="A129" s="2" t="s">
+      <c r="G128" s="25"/>
+      <c r="H128" s="24"/>
+    </row>
+    <row r="129" spans="3:7" ht="84">
+      <c r="C129" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D129" s="2" t="s">
+      <c r="F129" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E129" s="11" t="s">
+      <c r="G129" s="11" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="84">
-      <c r="A130" s="2" t="s">
+    <row r="130" spans="3:7" ht="84">
+      <c r="C130" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D130" s="2" t="s">
+      <c r="F130" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E130" s="11" t="s">
+      <c r="G130" s="11" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="84">
-      <c r="A131" s="2" t="s">
+    <row r="131" spans="3:7" ht="84">
+      <c r="C131" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D131" s="26" t="s">
+      <c r="F131" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E131" s="11" t="s">
+      <c r="G131" s="11" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="84">
-      <c r="A132" s="2" t="s">
+    <row r="132" spans="3:7" ht="84">
+      <c r="C132" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="D132" s="26" t="s">
+      <c r="F132" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E132" s="11" t="s">
+      <c r="G132" s="11" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="84">
-      <c r="A133" s="2" t="s">
+    <row r="133" spans="3:7" ht="84">
+      <c r="C133" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D133" s="26" t="s">
+      <c r="F133" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E133" s="11" t="s">
+      <c r="G133" s="11" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="84">
-      <c r="A134" s="2" t="s">
+    <row r="134" spans="3:7" ht="84">
+      <c r="C134" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D134" s="26" t="s">
+      <c r="F134" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E134" s="11" t="s">
+      <c r="G134" s="11" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="84">
-      <c r="A135" s="2" t="s">
+    <row r="135" spans="3:7" ht="84">
+      <c r="C135" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D135" s="2" t="s">
+      <c r="F135" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="E135" s="11" t="s">
+      <c r="G135" s="11" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="84">
-      <c r="A136" s="2" t="s">
+    <row r="136" spans="3:7" ht="84">
+      <c r="C136" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="D136" s="26" t="s">
+      <c r="F136" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E136" s="11" t="s">
+      <c r="G136" s="11" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="84">
-      <c r="A137" s="2" t="s">
+    <row r="137" spans="3:7" ht="84">
+      <c r="C137" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D137" s="26" t="s">
+      <c r="F137" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E137" s="11" t="s">
+      <c r="G137" s="11" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="84">
-      <c r="A138" s="2" t="s">
+    <row r="138" spans="3:7" ht="84">
+      <c r="C138" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="D138" s="26" t="s">
+      <c r="F138" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E138" s="11" t="s">
+      <c r="G138" s="11" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="84">
-      <c r="A139" s="2" t="s">
+    <row r="139" spans="3:7" ht="84">
+      <c r="C139" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D139" s="26" t="s">
+      <c r="F139" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="E139" s="11" t="s">
+      <c r="G139" s="11" t="s">
         <v>349</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SSP update for new VT LicenseCategoryCodeText and IncidentFactorText
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="1320" windowWidth="22280" windowHeight="15920"/>
+    <workbookView xWindow="5180" yWindow="2120" windowWidth="27920" windowHeight="15920"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="427">
   <si>
     <t>Description</t>
   </si>
@@ -1292,250 +1292,31 @@
     <t>Municipality Ordinance</t>
   </si>
   <si>
-    <t>Spillman</t>
-  </si>
-  <si>
-    <t>CTMAIN TABLE/ CTMDESC.TEXT</t>
-  </si>
-  <si>
-    <t>CTMAIN TABLE/CTMDESC.TEXT</t>
-  </si>
-  <si>
-    <t>NMMAIN.DLNUMB</t>
-  </si>
-  <si>
-    <t>NMLOCAL.LOCALID</t>
-  </si>
-  <si>
-    <t>NMMAIN.LAST</t>
-  </si>
-  <si>
-    <t>NMMAIN.FIRST</t>
-  </si>
-  <si>
-    <t>NMMAIN.MIDDLE</t>
-  </si>
-  <si>
-    <t>CTMAIN TABLE/ CTMDESC.TEXT (may need to change the form in TRACS so officer can signify that the mailing adddress is also the physical address. If it's different , we may need to add a physical address field in TraCS)</t>
-  </si>
-  <si>
-    <t>NMMAIN.PHONE</t>
-  </si>
-  <si>
-    <t>NMMAIN.WRKPHN</t>
-  </si>
-  <si>
-    <t>NMMAIN.BIRTHD</t>
-  </si>
-  <si>
-    <t>NMMAIN.SEX</t>
-  </si>
-  <si>
-    <t>NMEXTRA.BCITY</t>
-  </si>
-  <si>
-    <t>NMMAIN.HEIGHT</t>
-  </si>
-  <si>
-    <t>NMMAIN.WEIGHT</t>
-  </si>
-  <si>
-    <t>NMMAIN.HAIR</t>
-  </si>
-  <si>
-    <t>NNMAIN.EYES</t>
-  </si>
-  <si>
-    <t>VHMAIN.LPST</t>
-  </si>
-  <si>
-    <t>VHMAIN.YEAR</t>
-  </si>
-  <si>
-    <t>VHMAIN.MAKE</t>
-  </si>
-  <si>
-    <t>VHMAIN.MODEL</t>
-  </si>
-  <si>
-    <t>VHMAIN.COLOR1</t>
-  </si>
-  <si>
-    <t>CTMAIN.VILDATE</t>
-  </si>
-  <si>
     <t>Citation Violation Date/Time</t>
   </si>
   <si>
-    <t>CTMAIN.AGENCY</t>
-  </si>
-  <si>
-    <t>CTMAIN.STREET</t>
-  </si>
-  <si>
-    <t>CTMAIN.SPACT</t>
-  </si>
-  <si>
-    <t>CTMAIN.SPPOST</t>
-  </si>
-  <si>
-    <t>CTMAIN.ISSUOFF</t>
-  </si>
-  <si>
-    <t>CTMAIN.BONDAMT</t>
-  </si>
-  <si>
-    <t>CTMAIN.DTISSUE</t>
-  </si>
-  <si>
-    <t>MasterCitationTable/CitationNumber</t>
-  </si>
-  <si>
-    <t>MasterCitationTable/DateOfCitation</t>
-  </si>
-  <si>
-    <t>MasterCitationTable/BondAmount</t>
-  </si>
-  <si>
-    <t>CommentsForCitationRecords/MiscellaneousComments</t>
-  </si>
-  <si>
-    <t>MasterCitationTable/AgencyCode</t>
-  </si>
-  <si>
-    <t>MasterCitationTable/StreetAddress</t>
-  </si>
-  <si>
-    <t>MainNamesTable/LastName</t>
-  </si>
-  <si>
-    <t>MainNamesTable/FirstName</t>
-  </si>
-  <si>
-    <t>MainNamesTable/MiddleName</t>
-  </si>
-  <si>
-    <t>MainNamesTable/StreetAddress</t>
-  </si>
-  <si>
-    <t>MainNamesTable/CityOfResidence</t>
-  </si>
-  <si>
-    <t>MainNamesTable/StateAbbreviation</t>
-  </si>
-  <si>
-    <t>MainNamesTable/ZipCode</t>
-  </si>
-  <si>
-    <t>MainNamesTable/DriverLicenseNumber</t>
-  </si>
-  <si>
-    <t>MainNamesTable/DriverLicenseState</t>
-  </si>
-  <si>
-    <t>NMMAIN.DLSTATE</t>
-  </si>
-  <si>
-    <t>NameLocalIDDetail/LocalIDNumber</t>
-  </si>
-  <si>
-    <t>MainNamesTable/HomePhoneNumber</t>
-  </si>
-  <si>
-    <t>MainNamesTable/WorkTelephoneNumber</t>
-  </si>
-  <si>
-    <t>MainNamesTable/BirthDate</t>
-  </si>
-  <si>
-    <t>MainNamesTable/Sex</t>
-  </si>
-  <si>
-    <t>AdditionalNameInformation/CityOfBirth</t>
-  </si>
-  <si>
-    <t>MainNamesTable/Height</t>
-  </si>
-  <si>
-    <t>MainNamesTable/Weight</t>
-  </si>
-  <si>
-    <t>MainNamesTable/Hair</t>
-  </si>
-  <si>
-    <t>MainNamesTable/Eye</t>
-  </si>
-  <si>
-    <t>MainVehicleScreen/LicensePlateNumber</t>
-  </si>
-  <si>
-    <t>VHMAIN.LPNUM</t>
-  </si>
-  <si>
-    <t>MainVehicleScreen/LicenseStateAbbreviation</t>
-  </si>
-  <si>
-    <t>MainVehicleScreen/YearOfCar</t>
-  </si>
-  <si>
-    <t>MainVehicleScreen/MakeOfCar</t>
-  </si>
-  <si>
-    <t>MainVehicleScreen/ModelOfCar</t>
-  </si>
-  <si>
-    <t>MainVehicleScreen/ColorPrimary</t>
-  </si>
-  <si>
-    <t>MasterCitationTable/Posted</t>
-  </si>
-  <si>
-    <t>MasterCitationTable/Actual</t>
-  </si>
-  <si>
-    <t>MasterCitationTable/IssuingOfficer</t>
-  </si>
-  <si>
-    <t>MasterCitationTable/ViolationDate</t>
-  </si>
-  <si>
-    <t>LawIncidentTable/IncidentNumber</t>
-  </si>
-  <si>
-    <t>LWMAIN.NUMBER</t>
-  </si>
-  <si>
-    <t>LawIncidentTable/TimeDateOccurredAfter</t>
-  </si>
-  <si>
-    <t>LWMAIN.OCURDT1</t>
-  </si>
-  <si>
-    <t>LawIncidentTable/TimeDateOccurredBefore</t>
-  </si>
-  <si>
-    <t>LWMAIN.OCURDT2</t>
-  </si>
-  <si>
-    <t>LawIncidentNarrative/Narrative</t>
-  </si>
-  <si>
-    <t>LWNARR.NARRATV</t>
-  </si>
-  <si>
-    <t>LawIncidentTable/City</t>
-  </si>
-  <si>
-    <t>LWMAIN.CITY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTMAIN.NUMBER </t>
-  </si>
-  <si>
-    <t>varname</t>
-  </si>
-  <si>
-    <t>Tag</t>
+    <t>A category of a drivers license</t>
+  </si>
+  <si>
+    <t>Driver License Type (Spillman XML)</t>
+  </si>
+  <si>
+    <t>Driver License Category</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DriverLicense[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/@s:id]/inc-ext:DriverLicenseCategoryCodeText</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>Circumstance Code</t>
+  </si>
+  <si>
+    <t>I89</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Offense[ndexia:ActivityAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Offense']/@s:id]/j:IncidentFactor/j:IncidentFactorText</t>
   </si>
 </sst>
 </file>
@@ -1545,7 +1326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1663,35 +1444,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <strike/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <strike/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1705,7 +1457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1808,18 +1560,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2666,7 +2406,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2749,43 +2489,16 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3922,2623 +3635,2133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H139"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="D84" sqref="D84:D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="39.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="105.83203125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="57.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.1640625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="45.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="105.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="57.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.1640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="18">
-      <c r="A1" s="29" t="s">
-        <v>418</v>
-      </c>
-      <c r="B1" s="29"/>
+    <row r="1" spans="1:6" s="9" customFormat="1" ht="18">
+      <c r="A1" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="18" t="s">
-        <v>257</v>
+        <v>169</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="15" t="s">
-        <v>498</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>499</v>
-      </c>
-      <c r="C2" s="16" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="16" t="s">
         <v>73</v>
       </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="E2" s="12"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" ht="70">
-      <c r="A3" s="32" t="s">
-        <v>497</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>450</v>
+    </row>
+    <row r="3" spans="1:6" ht="70">
+      <c r="A3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="D3" s="2">
         <v>82734800</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A4" s="32" t="s">
-        <v>449</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>451</v>
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A4" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A5" s="32" t="s">
-        <v>441</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>486</v>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A5" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>411</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="E5" s="3" t="s">
         <v>412</v>
       </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="11" t="s">
+        <v>413</v>
+      </c>
       <c r="F5" s="7"/>
-      <c r="G5" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A6" s="32" t="s">
-        <v>448</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>452</v>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="27" t="s">
+      <c r="D6" s="27" t="s">
         <v>379</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A7" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>453</v>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A7" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7" s="27" t="s">
+      <c r="D7" s="27" t="s">
         <v>362</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A8" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>453</v>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A8" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F8" s="27" t="s">
+      <c r="D8" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="16" t="s">
         <v>216</v>
       </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="E9" s="12"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" ht="112" customHeight="1">
-      <c r="A10" s="33" t="s">
-        <v>443</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>454</v>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="112" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A11" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>453</v>
+    <row r="11" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A12" s="32" t="s">
-        <v>444</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>455</v>
+    <row r="12" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="15" t="s">
         <v>56</v>
       </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="E13" s="13"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="70">
-      <c r="A14" s="33" t="s">
-        <v>423</v>
-      </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="17" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="70">
+      <c r="A14" s="17" t="s">
         <v>3</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>223</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F14" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="84">
-      <c r="C15" s="20" t="s">
+    <row r="15" spans="1:6" ht="84">
+      <c r="A15" s="20" t="s">
         <v>51</v>
       </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="84">
+      <c r="A16" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="84">
+      <c r="A17" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3">
+        <v>5495</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="84">
+      <c r="A19" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D19" s="2">
+        <v>11846050</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="84">
+      <c r="A20" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A21" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="70">
+      <c r="A23" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="70">
+      <c r="A25" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="70">
+      <c r="A27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="70">
+      <c r="A28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="70">
+      <c r="A29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="112">
+      <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="B30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="84">
-      <c r="C16" s="20" t="s">
+      <c r="D30" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="112">
+      <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="84">
-      <c r="C17" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" ht="84">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="3">
-        <v>5495</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="84">
-      <c r="C19" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F19" s="2">
-        <v>11846050</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="84">
-      <c r="C20" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" ht="84">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="70">
-      <c r="A23" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" ht="70">
-      <c r="A25" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" ht="70">
-      <c r="A27" s="33" t="s">
-        <v>423</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>456</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="70">
-      <c r="A28" s="33" t="s">
-        <v>424</v>
-      </c>
-      <c r="B28" s="33" t="s">
-        <v>457</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="70">
-      <c r="A29" s="33" t="s">
-        <v>425</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>458</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="112">
-      <c r="A30" s="39" t="s">
-        <v>426</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>459</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="112">
-      <c r="A31" s="39" t="s">
-        <v>419</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>460</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="140">
-      <c r="A32" s="39" t="s">
-        <v>419</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>461</v>
+    <row r="32" spans="1:6" ht="140">
+      <c r="A32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="3" customFormat="1" ht="112">
-      <c r="A33" s="39" t="s">
-        <v>419</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>462</v>
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="3">
+      <c r="D33" s="3">
         <v>5401</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="E33" s="11" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="84">
-      <c r="A34" s="32" t="s">
+    <row r="34" spans="1:6" ht="84">
+      <c r="A34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1209345</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="84">
+      <c r="A35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="70">
+      <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="70">
+      <c r="A37" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="B34" s="33" t="s">
-        <v>463</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1209345</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="84">
-      <c r="A35" s="32" t="s">
-        <v>465</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>464</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="140">
+      <c r="A38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="2">
+        <v>12345678</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="7">
+        <v>24092</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A43" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="3">
+        <v>70</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A45" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A46" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="3">
+        <v>135</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A47" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A48" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A49" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A52" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="3" customFormat="1" ht="112">
+      <c r="A53" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="14" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="70">
-      <c r="A36" s="9" t="s">
-        <v>420</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="140">
-      <c r="A37" s="33" t="s">
-        <v>422</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>466</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="2">
-        <v>12345678</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="3" customFormat="1" ht="112">
-      <c r="A38" s="33" t="s">
-        <v>427</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>467</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="3" customFormat="1" ht="112">
-      <c r="A39" s="33" t="s">
-        <v>428</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>468</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A40" s="33" t="s">
-        <v>429</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="7">
-        <v>24092</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A41" s="33" t="s">
-        <v>430</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="3" customFormat="1" ht="84">
-      <c r="A42" s="33" t="s">
-        <v>431</v>
-      </c>
-      <c r="B42" s="33" t="s">
-        <v>471</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A43" s="33" t="s">
-        <v>432</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>472</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="3">
-        <v>70</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A45" s="33" t="s">
-        <v>433</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>473</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="3">
-        <v>135</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A47" s="33" t="s">
-        <v>434</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A48" s="33" t="s">
-        <v>435</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>475</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" s="3" customFormat="1" ht="98">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="3" customFormat="1" ht="112">
-      <c r="A51" s="33" t="s">
-        <v>477</v>
-      </c>
-      <c r="B51" s="33" t="s">
-        <v>476</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="3" customFormat="1" ht="112">
-      <c r="A52" s="33" t="s">
-        <v>436</v>
-      </c>
-      <c r="B52" s="33" t="s">
-        <v>478</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G52" s="11" t="s">
+      <c r="E53" s="11" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="3" customFormat="1" ht="98">
-      <c r="A53" s="33" t="s">
-        <v>437</v>
-      </c>
-      <c r="B53" s="33" t="s">
-        <v>479</v>
-      </c>
-      <c r="C53" s="3" t="s">
+    <row r="54" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A54" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="3">
+      <c r="D54" s="3">
         <v>2015</v>
       </c>
-      <c r="G53" s="11" t="s">
+      <c r="E54" s="11" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="3" customFormat="1" ht="98">
-      <c r="A54" s="33" t="s">
-        <v>438</v>
-      </c>
-      <c r="B54" s="33" t="s">
-        <v>480</v>
-      </c>
-      <c r="C54" s="3" t="s">
+    <row r="55" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A55" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="E55" s="11" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="3" customFormat="1" ht="98">
-      <c r="A55" s="33" t="s">
-        <v>439</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="C55" s="3" t="s">
+    <row r="56" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A56" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="E56" s="11" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="3" customFormat="1" ht="98">
-      <c r="A56" s="33" t="s">
-        <v>440</v>
-      </c>
-      <c r="B56" s="33" t="s">
-        <v>482</v>
-      </c>
-      <c r="C56" s="3" t="s">
+    <row r="57" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A57" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G56" s="11" t="s">
+      <c r="E57" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="3" customFormat="1" ht="98">
-      <c r="A57" s="31"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="3" t="s">
+    <row r="58" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A58" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="E58" s="11" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A58" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B58" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C58" s="3" t="s">
+    <row r="59" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A59" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F58" s="27" t="s">
+      <c r="D59" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="G58" s="11" t="s">
+      <c r="E59" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A59" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B59" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C59" s="3" t="s">
+    <row r="60" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A60" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F59" s="27" t="s">
+      <c r="D60" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="E60" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="15"/>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15" t="s">
+    <row r="61" spans="1:6">
+      <c r="A61" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="5"/>
-    </row>
-    <row r="61" spans="1:8" s="3" customFormat="1" ht="42">
-      <c r="A61" s="30" t="s">
-        <v>488</v>
-      </c>
-      <c r="B61" s="30" t="s">
-        <v>487</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A62" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G61" s="11" t="s">
+      <c r="E62" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="1:8" s="3" customFormat="1" ht="42">
-      <c r="A62" s="30" t="s">
-        <v>490</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>489</v>
-      </c>
-      <c r="C62" s="3" t="s">
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A63" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="F62" s="27" t="s">
+      <c r="D63" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="G62" s="11" t="s">
+      <c r="E63" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:8" s="3" customFormat="1" ht="42">
-      <c r="A63" s="30" t="s">
-        <v>492</v>
-      </c>
-      <c r="B63" s="30" t="s">
-        <v>491</v>
-      </c>
-      <c r="C63" s="3" t="s">
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A64" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F63" s="27" t="s">
+      <c r="D64" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="G63" s="11" t="s">
+      <c r="E64" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:8" s="35" customFormat="1" ht="70">
-      <c r="A64" s="40" t="s">
-        <v>494</v>
-      </c>
-      <c r="B64" s="34" t="s">
-        <v>493</v>
-      </c>
-      <c r="C64" s="35" t="s">
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" s="28" customFormat="1" ht="70">
+      <c r="A65" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D64" s="35" t="s">
+      <c r="B65" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E64" s="35" t="s">
+      <c r="C65" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="F64" s="36" t="s">
+      <c r="D65" s="29" t="s">
         <v>393</v>
       </c>
-      <c r="G64" s="37" t="s">
+      <c r="E65" s="30" t="s">
         <v>285</v>
       </c>
-      <c r="H64" s="38"/>
-    </row>
-    <row r="65" spans="1:7" s="3" customFormat="1" ht="126">
-      <c r="A65" s="33" t="s">
-        <v>496</v>
-      </c>
-      <c r="B65" s="30" t="s">
-        <v>495</v>
-      </c>
-      <c r="C65" s="3" t="s">
+      <c r="F65" s="31"/>
+    </row>
+    <row r="66" spans="1:6" s="3" customFormat="1" ht="126">
+      <c r="A66" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F65" s="27" t="s">
+      <c r="D66" s="27" t="s">
         <v>381</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="E66" s="11" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A66" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B66" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C66" s="3" t="s">
+    <row r="67" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A67" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F66" s="27" t="s">
+      <c r="D67" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="E67" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A67" s="32" t="s">
-        <v>444</v>
-      </c>
-      <c r="B67" s="32" t="s">
-        <v>455</v>
-      </c>
-      <c r="C67" s="3" t="s">
+    <row r="68" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A68" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F67" s="27" t="s">
+      <c r="D68" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="G67" s="11" t="s">
+      <c r="E68" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="3" customFormat="1" ht="42">
-      <c r="A68" s="33" t="s">
-        <v>494</v>
-      </c>
-      <c r="B68" s="30" t="s">
-        <v>493</v>
-      </c>
-      <c r="C68" s="3" t="s">
+    <row r="69" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A69" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F68" s="27" t="s">
+      <c r="D69" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="G68" s="11" t="s">
+      <c r="E69" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="3" customFormat="1" ht="98">
-      <c r="A69" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B69" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C69" s="3" t="s">
+    <row r="70" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A70" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F69" s="27">
+      <c r="D70" s="27">
         <v>0.2</v>
       </c>
-      <c r="G69" s="11" t="s">
+      <c r="E70" s="11" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A70" s="32" t="s">
-        <v>445</v>
-      </c>
-      <c r="B70" s="32" t="s">
-        <v>484</v>
-      </c>
-      <c r="C70" s="3" t="s">
+    <row r="71" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A71" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F70" s="27">
+      <c r="D71" s="27">
         <v>30</v>
       </c>
-      <c r="G70" s="11" t="s">
+      <c r="E71" s="11" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A71" s="31"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="3" t="s">
+    <row r="72" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A72" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F71" s="27" t="s">
+      <c r="D72" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="G71" s="11" t="s">
+      <c r="E72" s="11" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A72" s="32" t="s">
-        <v>446</v>
-      </c>
-      <c r="B72" s="32" t="s">
-        <v>483</v>
-      </c>
-      <c r="C72" s="3" t="s">
+    <row r="73" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A73" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F72" s="27">
+      <c r="D73" s="27">
         <v>40</v>
       </c>
-      <c r="G72" s="11" t="s">
+      <c r="E73" s="11" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A73" s="31"/>
-      <c r="B73" s="31"/>
-      <c r="C73" s="3" t="s">
+    <row r="74" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A74" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F73" s="27" t="s">
+      <c r="D74" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="G73" s="11" t="s">
+      <c r="E74" s="11" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A74" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B74" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C74" s="3" t="s">
+    <row r="75" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A75" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F74" s="27" t="s">
+      <c r="D75" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="G74" s="11" t="s">
+      <c r="E75" s="11" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A75" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B75" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C75" s="3" t="s">
+    <row r="76" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A76" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F75" s="27" t="s">
+      <c r="D76" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="G75" s="11" t="s">
+      <c r="E76" s="11" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A76" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B76" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C76" s="3" t="s">
+    <row r="77" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A77" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F76" s="27" t="s">
+      <c r="D77" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="G76" s="11" t="s">
+      <c r="E77" s="11" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="3" customFormat="1" ht="70">
-      <c r="A77" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B77" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C77" s="3" t="s">
+    <row r="78" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A78" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="F77" s="27" t="s">
+      <c r="D78" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="G77" s="11" t="s">
+      <c r="E78" s="11" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="70">
-      <c r="A78" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B78" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C78" s="2" t="s">
+    <row r="79" spans="1:6" ht="70">
+      <c r="A79" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F78" s="26" t="s">
+      <c r="D79" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G78" s="11" t="s">
+      <c r="E79" s="11" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="70">
-      <c r="A79" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B79" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C79" s="2" t="s">
+    <row r="80" spans="1:6" ht="70">
+      <c r="A80" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F79" s="26" t="s">
+      <c r="D80" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G79" s="11" t="s">
+      <c r="E80" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="70">
-      <c r="A80" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B80" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C80" s="2" t="s">
+    <row r="81" spans="1:6" ht="70">
+      <c r="A81" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F80" s="26" t="s">
+      <c r="D81" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G80" s="11" t="s">
+      <c r="E81" s="11" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="70">
-      <c r="A81" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B81" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C81" s="2" t="s">
+    <row r="82" spans="1:6" ht="70">
+      <c r="A82" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F81" s="26" t="s">
+      <c r="D82" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G81" s="11" t="s">
+      <c r="E82" s="11" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="15"/>
-      <c r="B82" s="15"/>
-      <c r="C82" s="15" t="s">
+    <row r="83" spans="1:6">
+      <c r="A83" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="5"/>
-    </row>
-    <row r="83" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A83" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B83" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C83" s="3" t="s">
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A84" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>417</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="F83" s="28" t="s">
-        <v>415</v>
-      </c>
-      <c r="G83" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" s="3" customFormat="1" ht="84">
-      <c r="A84" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B84" s="33" t="s">
-        <v>453</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>278</v>
       </c>
       <c r="D84" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A85" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F84" s="28" t="s">
+      <c r="C85" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G84" s="11" t="s">
+      <c r="E85" s="11" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A85" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B85" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C85" s="3" t="s">
+    <row r="86" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A86" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="B86" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E85" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F85" s="28" t="s">
+      <c r="D86" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G85" s="11" t="s">
+      <c r="E86" s="11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A86" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B86" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C86" s="3" t="s">
+    <row r="87" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A87" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E86" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="F86" s="28" t="s">
+      <c r="D87" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="G86" s="11" t="s">
+      <c r="E87" s="11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="3" customFormat="1" ht="98">
-      <c r="A87" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B87" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C87" s="3" t="s">
+    <row r="88" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A88" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="F87" s="3" t="s">
+      <c r="D88" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="G87" s="11" t="s">
+      <c r="E88" s="11" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="3" customFormat="1" ht="42">
-      <c r="A88" s="9" t="s">
-        <v>419</v>
-      </c>
-      <c r="B88" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C88" s="3" t="s">
+    <row r="89" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A89" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F88" s="27" t="s">
+      <c r="D89" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="G88" s="11" t="s">
+      <c r="E89" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="H88" s="6"/>
-    </row>
-    <row r="89" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A89" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B89" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C89" s="3" t="s">
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A90" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F89" s="27">
+      <c r="D90" s="27">
         <v>2</v>
       </c>
-      <c r="G89" s="11" t="s">
+      <c r="E90" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A90" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B90" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C90" s="3" t="s">
+    <row r="91" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A91" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F90" s="27" t="s">
+      <c r="D91" s="27" t="s">
         <v>395</v>
       </c>
-      <c r="G90" s="11" t="s">
+      <c r="E91" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="H90" s="8"/>
-    </row>
-    <row r="91" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A91" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B91" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C91" s="3" t="s">
+      <c r="F91" s="8"/>
+    </row>
+    <row r="92" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A92" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="C92" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F91" s="27" t="s">
+      <c r="D92" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="G91" s="11" t="s">
+      <c r="E92" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="H91" s="8"/>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="15"/>
-      <c r="B92" s="15"/>
-      <c r="C92" s="15" t="s">
+      <c r="F92" s="8"/>
+    </row>
+    <row r="93" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A93" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D93" s="27" t="s">
+        <v>425</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="F93" s="8"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="5"/>
-    </row>
-    <row r="93" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A93" s="32" t="s">
-        <v>447</v>
-      </c>
-      <c r="B93" s="32" t="s">
-        <v>485</v>
-      </c>
-      <c r="C93" s="3" t="s">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A95" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="B95" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F93" s="3" t="s">
+      <c r="D95" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G93" s="11" t="s">
+      <c r="E95" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="94" spans="1:8" s="3" customFormat="1" ht="42">
-      <c r="A94" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B94" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C94" s="3" t="s">
+    <row r="96" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A96" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E94" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="F94" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="G94" s="11" t="s">
+      <c r="E96" s="11" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="3" customFormat="1" ht="84">
-      <c r="A95" s="9" t="s">
-        <v>419</v>
-      </c>
-      <c r="B95" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C95" s="3" t="s">
+    <row r="97" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A97" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F95" s="3">
+      <c r="D97" s="3">
         <v>12345</v>
       </c>
-      <c r="G95" s="11" t="s">
+      <c r="E97" s="11" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="3" customFormat="1" ht="84">
-      <c r="A96" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B96" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C96" s="3" t="s">
+    <row r="98" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A98" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="B98" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="C98" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F96" s="3" t="s">
+      <c r="D98" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="G96" s="11" t="s">
+      <c r="E98" s="11" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A97" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B97" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C97" s="3" t="s">
+    <row r="99" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A99" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F97" s="3" t="s">
+      <c r="D99" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G97" s="11" t="s">
+      <c r="E99" s="11" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
-      <c r="A98" s="15"/>
-      <c r="B98" s="15"/>
-      <c r="C98" s="15" t="s">
+    <row r="100" spans="1:6">
+      <c r="A100" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="5"/>
-    </row>
-    <row r="99" spans="1:8" ht="70">
-      <c r="A99" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B99" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C99" s="3" t="s">
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" ht="70">
+      <c r="A101" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="C101" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F99" s="3" t="s">
+      <c r="D101" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G99" s="10" t="s">
+      <c r="E101" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="H99" s="3"/>
-    </row>
-    <row r="100" spans="1:8" ht="70">
-      <c r="A100" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B100" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C100" s="2" t="s">
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:6" ht="70">
+      <c r="A102" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="D102" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G100" s="10" t="s">
+      <c r="E102" s="10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="112">
-      <c r="A101" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B101" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C101" s="3" t="s">
+    <row r="103" spans="1:6" ht="112">
+      <c r="A103" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="C103" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F101" s="3" t="s">
+      <c r="D103" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G101" s="10" t="s">
+      <c r="E103" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="H101" s="3"/>
-    </row>
-    <row r="102" spans="1:8" ht="112">
-      <c r="A102" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B102" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C102" s="3" t="s">
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="1:6" ht="112">
+      <c r="A104" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F102" s="3" t="s">
+      <c r="D104" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G102" s="10" t="s">
+      <c r="E104" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="H102" s="3"/>
-    </row>
-    <row r="103" spans="1:8" ht="126">
-      <c r="A103" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B103" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C103" s="3" t="s">
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="1:6" ht="126">
+      <c r="A105" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F103" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G103" s="10" t="s">
+      <c r="E105" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="H103" s="3"/>
-    </row>
-    <row r="104" spans="1:8" ht="112">
-      <c r="A104" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="B104" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C104" s="3" t="s">
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" ht="112">
+      <c r="A106" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F104" s="3" t="s">
+      <c r="D106" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G104" s="10" t="s">
+      <c r="E106" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="H104" s="3"/>
-    </row>
-    <row r="105" spans="1:8" ht="31" customHeight="1">
-      <c r="C105" s="23" t="s">
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:6" ht="31" customHeight="1">
+      <c r="A107" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="D105" s="21"/>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="22"/>
-      <c r="H105" s="21"/>
-    </row>
-    <row r="106" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A106" s="30"/>
-      <c r="B106" s="30"/>
-      <c r="C106" s="3" t="s">
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="21"/>
+    </row>
+    <row r="108" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A108" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="F106" s="3" t="s">
+      <c r="D108" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="G106" s="14" t="s">
+      <c r="E108" s="14" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="107" spans="1:8" s="3" customFormat="1" ht="70">
-      <c r="A107" s="30"/>
-      <c r="B107" s="30"/>
-      <c r="C107" s="3" t="s">
+    <row r="109" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A109" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="F107" s="3" t="s">
+      <c r="D109" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="G107" s="11" t="s">
+      <c r="E109" s="11" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="70">
-      <c r="C108" s="2" t="s">
+    <row r="110" spans="1:6" ht="70">
+      <c r="A110" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="D110" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="G108" s="11" t="s">
+      <c r="E110" s="11" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="70">
-      <c r="C109" s="2" t="s">
+    <row r="111" spans="1:6" ht="70">
+      <c r="A111" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="G109" s="11" t="s">
+      <c r="E111" s="11" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="70">
-      <c r="C110" s="2" t="s">
+    <row r="112" spans="1:6" ht="70">
+      <c r="A112" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="D112" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="G110" s="11" t="s">
+      <c r="E112" s="11" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="70">
-      <c r="C111" s="2" t="s">
+    <row r="113" spans="1:6" ht="70">
+      <c r="A113" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="D113" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="G111" s="11" t="s">
+      <c r="E113" s="11" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="70">
-      <c r="C112" s="2" t="s">
+    <row r="114" spans="1:6" ht="70">
+      <c r="A114" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="D114" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="G112" s="11" t="s">
+      <c r="E114" s="11" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="113" spans="3:8" ht="70">
-      <c r="C113" s="2" t="s">
+    <row r="115" spans="1:6" ht="70">
+      <c r="A115" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="D115" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="G113" s="11" t="s">
+      <c r="E115" s="11" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="114" spans="3:8" ht="70">
-      <c r="C114" s="2" t="s">
+    <row r="116" spans="1:6" ht="70">
+      <c r="A116" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="D116" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="G114" s="11" t="s">
+      <c r="E116" s="11" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="115" spans="3:8" ht="70">
-      <c r="C115" s="2" t="s">
+    <row r="117" spans="1:6" ht="70">
+      <c r="A117" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="D117" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="G115" s="11" t="s">
+      <c r="E117" s="11" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="116" spans="3:8" ht="14" customHeight="1">
-      <c r="C116" s="24" t="s">
+    <row r="118" spans="1:6" ht="14" customHeight="1">
+      <c r="A118" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="D116" s="24"/>
-      <c r="E116" s="24"/>
-      <c r="F116" s="24"/>
-      <c r="G116" s="25"/>
-      <c r="H116" s="24"/>
-    </row>
-    <row r="117" spans="3:8" ht="73" customHeight="1">
-      <c r="C117" s="2" t="s">
+      <c r="B118" s="24"/>
+      <c r="C118" s="24"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="25"/>
+      <c r="F118" s="24"/>
+    </row>
+    <row r="119" spans="1:6" ht="73" customHeight="1">
+      <c r="A119" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="D119" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="G117" s="11" t="s">
+      <c r="E119" s="11" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="118" spans="3:8" ht="84">
-      <c r="C118" s="2" t="s">
+    <row r="120" spans="1:6" ht="84">
+      <c r="A120" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="D120" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="G118" s="11" t="s">
+      <c r="E120" s="11" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="119" spans="3:8" ht="84">
-      <c r="C119" s="2" t="s">
+    <row r="121" spans="1:6" ht="84">
+      <c r="A121" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F119" s="26" t="s">
+      <c r="D121" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G119" s="11" t="s">
+      <c r="E121" s="11" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="120" spans="3:8" ht="84">
-      <c r="C120" s="2" t="s">
+    <row r="122" spans="1:6" ht="84">
+      <c r="A122" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F120" s="26" t="s">
+      <c r="D122" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G120" s="11" t="s">
+      <c r="E122" s="11" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="121" spans="3:8" ht="84">
-      <c r="C121" s="2" t="s">
+    <row r="123" spans="1:6" ht="84">
+      <c r="A123" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="F121" s="26" t="s">
+      <c r="D123" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G121" s="11" t="s">
+      <c r="E123" s="11" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="122" spans="3:8" ht="84">
-      <c r="C122" s="2" t="s">
+    <row r="124" spans="1:6" ht="84">
+      <c r="A124" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F122" s="26" t="s">
+      <c r="D124" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G122" s="11" t="s">
+      <c r="E124" s="11" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="123" spans="3:8" ht="84">
-      <c r="C123" s="2" t="s">
+    <row r="125" spans="1:6" ht="84">
+      <c r="A125" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F123" s="2" t="s">
+      <c r="D125" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="G123" s="11" t="s">
+      <c r="E125" s="11" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="124" spans="3:8" ht="84">
-      <c r="C124" s="2" t="s">
+    <row r="126" spans="1:6" ht="84">
+      <c r="A126" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="F124" s="26" t="s">
+      <c r="D126" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G124" s="11" t="s">
+      <c r="E126" s="11" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="125" spans="3:8" ht="84">
-      <c r="C125" s="2" t="s">
+    <row r="127" spans="1:6" ht="84">
+      <c r="A127" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="F125" s="26" t="s">
+      <c r="D127" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G125" s="11" t="s">
+      <c r="E127" s="11" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="126" spans="3:8" ht="84">
-      <c r="C126" s="2" t="s">
+    <row r="128" spans="1:6" ht="84">
+      <c r="A128" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F126" s="26" t="s">
+      <c r="D128" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G126" s="11" t="s">
+      <c r="E128" s="11" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="127" spans="3:8" ht="84">
-      <c r="C127" s="2" t="s">
+    <row r="129" spans="1:6" ht="84">
+      <c r="A129" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="F127" s="26" t="s">
+      <c r="D129" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G127" s="11" t="s">
+      <c r="E129" s="11" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="128" spans="3:8" ht="14" customHeight="1">
-      <c r="C128" s="24" t="s">
+    <row r="130" spans="1:6" ht="14" customHeight="1">
+      <c r="A130" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="D128" s="24"/>
-      <c r="E128" s="24"/>
-      <c r="F128" s="24"/>
-      <c r="G128" s="25"/>
-      <c r="H128" s="24"/>
-    </row>
-    <row r="129" spans="3:7" ht="84">
-      <c r="C129" s="2" t="s">
+      <c r="B130" s="24"/>
+      <c r="C130" s="24"/>
+      <c r="D130" s="24"/>
+      <c r="E130" s="25"/>
+      <c r="F130" s="24"/>
+    </row>
+    <row r="131" spans="1:6" ht="84">
+      <c r="A131" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="F129" s="2" t="s">
+      <c r="D131" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="G129" s="11" t="s">
+      <c r="E131" s="11" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="130" spans="3:7" ht="84">
-      <c r="C130" s="2" t="s">
+    <row r="132" spans="1:6" ht="84">
+      <c r="A132" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="F130" s="2" t="s">
+      <c r="D132" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="G130" s="11" t="s">
+      <c r="E132" s="11" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="131" spans="3:7" ht="84">
-      <c r="C131" s="2" t="s">
+    <row r="133" spans="1:6" ht="84">
+      <c r="A133" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="F131" s="26" t="s">
+      <c r="D133" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G131" s="11" t="s">
+      <c r="E133" s="11" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="132" spans="3:7" ht="84">
-      <c r="C132" s="2" t="s">
+    <row r="134" spans="1:6" ht="84">
+      <c r="A134" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="F132" s="26" t="s">
+      <c r="D134" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G132" s="11" t="s">
+      <c r="E134" s="11" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="133" spans="3:7" ht="84">
-      <c r="C133" s="2" t="s">
+    <row r="135" spans="1:6" ht="84">
+      <c r="A135" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F133" s="26" t="s">
+      <c r="D135" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G133" s="11" t="s">
+      <c r="E135" s="11" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="134" spans="3:7" ht="84">
-      <c r="C134" s="2" t="s">
+    <row r="136" spans="1:6" ht="84">
+      <c r="A136" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="F134" s="26" t="s">
+      <c r="D136" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G134" s="11" t="s">
+      <c r="E136" s="11" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="135" spans="3:7" ht="84">
-      <c r="C135" s="2" t="s">
+    <row r="137" spans="1:6" ht="84">
+      <c r="A137" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F135" s="2" t="s">
+      <c r="D137" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="G135" s="11" t="s">
+      <c r="E137" s="11" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="136" spans="3:7" ht="84">
-      <c r="C136" s="2" t="s">
+    <row r="138" spans="1:6" ht="84">
+      <c r="A138" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="F136" s="26" t="s">
+      <c r="D138" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G136" s="11" t="s">
+      <c r="E138" s="11" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="137" spans="3:7" ht="84">
-      <c r="C137" s="2" t="s">
+    <row r="139" spans="1:6" ht="84">
+      <c r="A139" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="F137" s="26" t="s">
+      <c r="D139" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G137" s="11" t="s">
+      <c r="E139" s="11" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="138" spans="3:7" ht="84">
-      <c r="C138" s="2" t="s">
+    <row r="140" spans="1:6" ht="84">
+      <c r="A140" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F138" s="26" t="s">
+      <c r="D140" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G138" s="11" t="s">
+      <c r="E140" s="11" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="139" spans="3:7" ht="84">
-      <c r="C139" s="2" t="s">
+    <row r="141" spans="1:6" ht="84">
+      <c r="A141" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="F139" s="26" t="s">
+      <c r="D141" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="G139" s="11" t="s">
+      <c r="E141" s="11" t="s">
         <v>349</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added License Plate Category Text element for VT eCitation
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Incident_Reporting/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/vermont/Incident_Citation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="2120" windowWidth="27920" windowHeight="15920"/>
+    <workbookView xWindow="5180" yWindow="2100" windowWidth="27920" windowHeight="15920"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -1295,18 +1295,6 @@
     <t>Citation Violation Date/Time</t>
   </si>
   <si>
-    <t>A category of a drivers license</t>
-  </si>
-  <si>
-    <t>Driver License Type (Spillman XML)</t>
-  </si>
-  <si>
-    <t>Driver License Category</t>
-  </si>
-  <si>
-    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DriverLicense[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person/@s:id]/inc-ext:DriverLicenseCategoryCodeText</t>
-  </si>
-  <si>
     <t>PO</t>
   </si>
   <si>
@@ -1317,6 +1305,18 @@
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/ndexia:IncidentReport/ndexia:Offense[ndexia:ActivityAugmentation/lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Offense']/@s:id]/j:IncidentFactor/j:IncidentFactorText</t>
+  </si>
+  <si>
+    <t>License Plate Category</t>
+  </si>
+  <si>
+    <t>A category of a license plate</t>
+  </si>
+  <si>
+    <t>License Plate Type (Spillman XML)</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Vehicle[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityVehicle/nc:Vehicle/@s:id]/nc:ConveyanceRegistrationPlateCategoryText</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1570,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="834">
+  <cellStyleXfs count="836">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1597,6 +1597,8 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2502,7 +2504,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="834">
+  <cellStyles count="836">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2928,6 +2930,7 @@
     <cellStyle name="Followed Hyperlink" xfId="829" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="831" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="833" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="835" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -3332,6 +3335,7 @@
     <cellStyle name="Hyperlink" xfId="828" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="830" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="832" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="834" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -3635,11 +3639,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F141"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D84" sqref="D84:D87"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4232,23 +4236,6 @@
         <v>281</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="70">
-      <c r="A37" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>422</v>
-      </c>
-    </row>
     <row r="38" spans="1:6" ht="140">
       <c r="A38" s="2" t="s">
         <v>80</v>
@@ -4628,1140 +4615,1157 @@
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="15" t="s">
+    <row r="61" spans="1:6" ht="70">
+      <c r="A61" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="5"/>
-    </row>
-    <row r="62" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A62" s="2" t="s">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A63" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E62" s="11" t="s">
+      <c r="E63" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A63" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D63" s="27" t="s">
-        <v>391</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="F63" s="7"/>
+      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A64" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>391</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A65" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D64" s="27" t="s">
+      <c r="D65" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="E65" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="F64" s="7"/>
-    </row>
-    <row r="65" spans="1:6" s="28" customFormat="1" ht="70">
-      <c r="A65" s="28" t="s">
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:6" s="28" customFormat="1" ht="70">
+      <c r="A66" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B65" s="28" t="s">
+      <c r="B66" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="28" t="s">
+      <c r="C66" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D65" s="29" t="s">
+      <c r="D66" s="29" t="s">
         <v>393</v>
       </c>
-      <c r="E65" s="30" t="s">
+      <c r="E66" s="30" t="s">
         <v>285</v>
       </c>
-      <c r="F65" s="31"/>
-    </row>
-    <row r="66" spans="1:6" s="3" customFormat="1" ht="126">
-      <c r="A66" s="3" t="s">
+      <c r="F66" s="31"/>
+    </row>
+    <row r="67" spans="1:6" s="3" customFormat="1" ht="126">
+      <c r="A67" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D66" s="27" t="s">
+      <c r="D67" s="27" t="s">
         <v>381</v>
       </c>
-      <c r="E66" s="11" t="s">
+      <c r="E67" s="11" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A67" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D67" s="27" t="s">
-        <v>382</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A68" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A69" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D68" s="27" t="s">
+      <c r="D69" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="E68" s="11" t="s">
+      <c r="E69" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A69" s="3" t="s">
+    <row r="70" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A70" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D69" s="27" t="s">
+      <c r="D70" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="E69" s="11" t="s">
+      <c r="E70" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A70" s="3" t="s">
+    <row r="71" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A71" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D70" s="27">
+      <c r="D71" s="27">
         <v>0.2</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="E71" s="11" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A71" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D71" s="27">
-        <v>30</v>
-      </c>
-      <c r="E71" s="11" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A72" s="3" t="s">
-        <v>144</v>
+        <v>33</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D72" s="27" t="s">
-        <v>145</v>
+        <v>62</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="27">
+        <v>30</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A73" s="3" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D73" s="27">
-        <v>40</v>
+        <v>167</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>145</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A74" s="3" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D74" s="27" t="s">
-        <v>145</v>
+        <v>63</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="27">
+        <v>40</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A75" s="3" t="s">
-        <v>100</v>
+        <v>144</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>35</v>
+        <v>168</v>
       </c>
       <c r="D75" s="27" t="s">
-        <v>380</v>
+        <v>145</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A76" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D76" s="27" t="s">
         <v>380</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A77" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D77" s="27" t="s">
         <v>380</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A78" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D78" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A79" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="D78" s="27" t="s">
+      <c r="D79" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="E79" s="11" t="s">
         <v>410</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="70">
-      <c r="A79" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D79" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="E79" s="11" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="70">
       <c r="A80" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D80" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="70">
       <c r="A81" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D81" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="70">
       <c r="A82" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="70">
+      <c r="A83" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D82" s="26" t="s">
+      <c r="D83" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="E82" s="11" t="s">
+      <c r="E83" s="11" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="15" t="s">
+    <row r="84" spans="1:6">
+      <c r="A84" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="5"/>
-    </row>
-    <row r="84" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A84" s="3" t="s">
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A85" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>417</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A85" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>278</v>
       </c>
       <c r="D85" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A86" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E85" s="11" t="s">
+      <c r="E86" s="11" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A86" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E86" s="11" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A87" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A88" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D88" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="E88" s="11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="88" spans="1:6" s="3" customFormat="1" ht="98">
-      <c r="A88" s="3" t="s">
+    <row r="89" spans="1:6" s="3" customFormat="1" ht="98">
+      <c r="A89" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D89" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="E88" s="11" t="s">
+      <c r="E89" s="11" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A89" s="3" t="s">
+    <row r="90" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A90" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D89" s="27" t="s">
+      <c r="D90" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="E89" s="11" t="s">
+      <c r="E90" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="F89" s="6"/>
-    </row>
-    <row r="90" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A90" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D90" s="27">
-        <v>2</v>
-      </c>
-      <c r="E90" s="11" t="s">
-        <v>183</v>
-      </c>
+      <c r="F90" s="6"/>
     </row>
     <row r="91" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A91" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D91" s="27" t="s">
-        <v>395</v>
+        <v>41</v>
+      </c>
+      <c r="D91" s="27">
+        <v>2</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="F91" s="8"/>
+        <v>183</v>
+      </c>
     </row>
     <row r="92" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A92" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D92" s="27" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F92" s="8"/>
     </row>
     <row r="93" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A93" s="3" t="s">
-        <v>424</v>
+        <v>109</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>424</v>
+        <v>72</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D93" s="27" t="s">
-        <v>425</v>
+        <v>396</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>426</v>
+        <v>185</v>
       </c>
       <c r="F93" s="8"/>
     </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="15" t="s">
+    <row r="94" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A94" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>421</v>
+      </c>
+      <c r="E94" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="F94" s="8"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="5"/>
-    </row>
-    <row r="95" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A95" s="3" t="s">
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A96" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E95" s="11" t="s">
+      <c r="E96" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="3" customFormat="1" ht="42">
-      <c r="A96" s="3" t="s">
+    <row r="97" spans="1:6" s="3" customFormat="1" ht="42">
+      <c r="A97" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D97" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="E96" s="11" t="s">
+      <c r="E97" s="11" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" s="3" customFormat="1" ht="84">
-      <c r="A97" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D97" s="3">
-        <v>12345</v>
-      </c>
-      <c r="E97" s="11" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A98" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D98" s="3">
+        <v>12345</v>
+      </c>
+      <c r="E98" s="11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" s="3" customFormat="1" ht="84">
+      <c r="A99" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D99" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E98" s="11" t="s">
+      <c r="E99" s="11" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A99" s="3" t="s">
+    <row r="100" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A100" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D100" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="E99" s="11" t="s">
+      <c r="E100" s="11" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="15" t="s">
+    <row r="101" spans="1:6">
+      <c r="A101" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B100" s="5"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="5"/>
-    </row>
-    <row r="101" spans="1:6" ht="70">
-      <c r="A101" s="3" t="s">
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="5"/>
+    </row>
+    <row r="102" spans="1:6" ht="70">
+      <c r="A102" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D102" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E101" s="10" t="s">
+      <c r="E102" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="F101" s="3"/>
-    </row>
-    <row r="102" spans="1:6" ht="70">
-      <c r="A102" s="2" t="s">
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="1:6" ht="70">
+      <c r="A103" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E102" s="10" t="s">
+      <c r="E103" s="10" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="112">
-      <c r="A103" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E103" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="F103" s="3"/>
     </row>
     <row r="104" spans="1:6" ht="112">
       <c r="A104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="1:6" ht="112">
+      <c r="A105" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E104" s="10" t="s">
+      <c r="E105" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="F104" s="3"/>
-    </row>
-    <row r="105" spans="1:6" ht="126">
-      <c r="A105" s="3" t="s">
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" ht="126">
+      <c r="A106" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B106" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D105" s="3" t="s">
+      <c r="D106" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E105" s="10" t="s">
+      <c r="E106" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="F105" s="3"/>
-    </row>
-    <row r="106" spans="1:6" ht="112">
-      <c r="A106" s="3" t="s">
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:6" ht="112">
+      <c r="A107" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D107" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E106" s="10" t="s">
+      <c r="E107" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="F106" s="3"/>
-    </row>
-    <row r="107" spans="1:6" ht="31" customHeight="1">
-      <c r="A107" s="23" t="s">
+      <c r="F107" s="3"/>
+    </row>
+    <row r="108" spans="1:6" ht="31" customHeight="1">
+      <c r="A108" s="23" t="s">
         <v>297</v>
       </c>
-      <c r="B107" s="21"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="21"/>
-      <c r="E107" s="22"/>
-      <c r="F107" s="21"/>
-    </row>
-    <row r="108" spans="1:6" s="3" customFormat="1" ht="70">
-      <c r="A108" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="E108" s="14" t="s">
-        <v>298</v>
-      </c>
+      <c r="B108" s="21"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="21"/>
+      <c r="E108" s="22"/>
+      <c r="F108" s="21"/>
     </row>
     <row r="109" spans="1:6" s="3" customFormat="1" ht="70">
       <c r="A109" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E109" s="14" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="3" customFormat="1" ht="70">
+      <c r="A110" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D110" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E109" s="11" t="s">
+      <c r="E110" s="11" t="s">
         <v>406</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="70">
-      <c r="A110" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="E110" s="11" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="70">
       <c r="A111" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="70">
       <c r="A112" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="70">
       <c r="A113" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="70">
       <c r="A114" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="70">
       <c r="A115" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E115" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="70">
       <c r="A116" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E116" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="70">
       <c r="A117" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E117" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="70">
+      <c r="A118" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="D118" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="E117" s="11" t="s">
+      <c r="E118" s="11" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="14" customHeight="1">
-      <c r="A118" s="24" t="s">
+    <row r="119" spans="1:6" ht="14" customHeight="1">
+      <c r="A119" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="B118" s="24"/>
-      <c r="C118" s="24"/>
-      <c r="D118" s="24"/>
-      <c r="E118" s="25"/>
-      <c r="F118" s="24"/>
-    </row>
-    <row r="119" spans="1:6" ht="73" customHeight="1">
-      <c r="A119" s="2" t="s">
+      <c r="B119" s="24"/>
+      <c r="C119" s="24"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="25"/>
+      <c r="F119" s="24"/>
+    </row>
+    <row r="120" spans="1:6" ht="73" customHeight="1">
+      <c r="A120" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="D120" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="E119" s="11" t="s">
+      <c r="E120" s="11" t="s">
         <v>334</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="84">
-      <c r="A120" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="E120" s="11" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="84">
       <c r="A121" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="D121" s="26" t="s">
-        <v>362</v>
+        <v>309</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="84">
       <c r="A122" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D122" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="84">
       <c r="A123" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D123" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="84">
       <c r="A124" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D124" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="84">
       <c r="A125" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>374</v>
+        <v>313</v>
+      </c>
+      <c r="D125" s="26" t="s">
+        <v>362</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="84">
       <c r="A126" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D126" s="26" t="s">
-        <v>362</v>
+        <v>314</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>374</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="84">
       <c r="A127" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D127" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E127" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="128" spans="1:6" ht="84">
       <c r="A128" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D128" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="84">
       <c r="A129" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D129" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E129" s="11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="84">
+      <c r="A130" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D130" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="E130" s="11" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="14" customHeight="1">
-      <c r="A130" s="24" t="s">
+    <row r="131" spans="1:6" ht="14" customHeight="1">
+      <c r="A131" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="B130" s="24"/>
-      <c r="C130" s="24"/>
-      <c r="D130" s="24"/>
-      <c r="E130" s="25"/>
-      <c r="F130" s="24"/>
-    </row>
-    <row r="131" spans="1:6" ht="84">
-      <c r="A131" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="E131" s="11" t="s">
-        <v>345</v>
-      </c>
+      <c r="B131" s="24"/>
+      <c r="C131" s="24"/>
+      <c r="D131" s="24"/>
+      <c r="E131" s="25"/>
+      <c r="F131" s="24"/>
     </row>
     <row r="132" spans="1:6" ht="84">
       <c r="A132" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="84">
       <c r="A133" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="D133" s="26" t="s">
-        <v>362</v>
+        <v>320</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="84">
       <c r="A134" s="2" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="D134" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="84">
       <c r="A135" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D135" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="84">
       <c r="A136" s="2" t="s">
-        <v>321</v>
+        <v>353</v>
       </c>
       <c r="D136" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E136" s="11" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="84">
       <c r="A137" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>376</v>
+        <v>321</v>
+      </c>
+      <c r="D137" s="26" t="s">
+        <v>362</v>
       </c>
       <c r="E137" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="84">
       <c r="A138" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="D138" s="26" t="s">
-        <v>362</v>
+        <v>322</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="84">
       <c r="A139" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D139" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E139" s="11" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="84">
       <c r="A140" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D140" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E140" s="11" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="84">
       <c r="A141" s="2" t="s">
-        <v>323</v>
+        <v>360</v>
       </c>
       <c r="D141" s="26" t="s">
         <v>362</v>
       </c>
       <c r="E141" s="11" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="84">
+      <c r="A142" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D142" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="E142" s="11" t="s">
         <v>349</v>
       </c>
     </row>

</xml_diff>